<commit_message>
Improve the Highlighter + the multiline control
</commit_message>
<xml_diff>
--- a/TestsAndDemos/Tests/Etk.Tests.Templates.ExcelDna1/Etk.Tests.Templates.ExcelDna1.xlsx
+++ b/TestsAndDemos/Tests/Etk.Tests.Templates.ExcelDna1/Etk.Tests.Templates.ExcelDna1.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="130">
   <si>
     <t>Basic vertical templates</t>
   </si>
@@ -365,18 +365,12 @@
     <t>{Success}</t>
   </si>
   <si>
-    <t>{Exception}</t>
-  </si>
-  <si>
     <t>{Done}</t>
   </si>
   <si>
     <t>Done</t>
   </si>
   <si>
-    <t>[Execute]</t>
-  </si>
-  <si>
     <t>[Execute All Tests]</t>
   </si>
   <si>
@@ -401,13 +395,28 @@
     <t>&lt;EndTemplate Name='Tests'/&gt;</t>
   </si>
   <si>
-    <t>{InitSuccessful}</t>
-  </si>
-  <si>
     <t>Init Ok</t>
   </si>
   <si>
     <t>{?Search...?}</t>
+  </si>
+  <si>
+    <t>[ME=ExcelTests,Etk.Tests.Templates.ExcelDna1,GetNumberOfTests:Execute]</t>
+  </si>
+  <si>
+    <t>{ME=ExcelTests,Etk.Tests.Templates.ExcelDna1,GetNumberOfTests:Description}</t>
+  </si>
+  <si>
+    <t>{ME=ExcelTests,Etk.Tests.Templates.ExcelDna1,GetNumberOfTests:InitSuccessful}</t>
+  </si>
+  <si>
+    <t>{ME=ExcelTests,Etk.Tests.Templates.ExcelDna1,GetNumberOfTests:Exception}</t>
+  </si>
+  <si>
+    <t>Errors</t>
+  </si>
+  <si>
+    <t>{Errors}</t>
   </si>
 </sst>
 </file>
@@ -451,8 +460,8 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0" tint="-4.9989318521683403E-2"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -460,12 +469,13 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="23">
+  <fills count="24">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -598,6 +608,16 @@
         <bgColor rgb="FF696969"/>
       </patternFill>
     </fill>
+    <fill>
+      <gradientFill degree="90">
+        <stop position="0">
+          <color theme="2" tint="-9.8025452436902985E-2"/>
+        </stop>
+        <stop position="1">
+          <color theme="2" tint="-0.74901577806939912"/>
+        </stop>
+      </gradientFill>
+    </fill>
   </fills>
   <borders count="24">
     <border>
@@ -990,10 +1010,6 @@
     <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="20" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1002,16 +1018,19 @@
     <xf numFmtId="0" fontId="0" fillId="22" borderId="0" xfId="0" applyFill="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="16" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="21" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1137,6 +1156,12 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFCC0000"/>
+      <color rgb="FFFFCCCC"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1434,85 +1459,85 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B2" s="41"/>
-      <c r="C2" s="42"/>
-      <c r="D2" s="42"/>
-      <c r="E2" s="42"/>
-      <c r="F2" s="42"/>
-      <c r="G2" s="42"/>
-      <c r="H2" s="42"/>
-      <c r="I2" s="42"/>
-      <c r="J2" s="42"/>
-      <c r="K2" s="42"/>
-      <c r="L2" s="41"/>
-      <c r="M2" s="41"/>
-      <c r="N2" s="43"/>
-      <c r="O2" s="43"/>
+      <c r="B2" s="40"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="41"/>
+      <c r="I2" s="41"/>
+      <c r="J2" s="41"/>
+      <c r="K2" s="41"/>
+      <c r="L2" s="40"/>
+      <c r="M2" s="40"/>
+      <c r="N2" s="42"/>
+      <c r="O2" s="42"/>
     </row>
     <row r="3" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B3" s="41"/>
-      <c r="C3" s="41"/>
-      <c r="D3" s="41"/>
-      <c r="E3" s="41"/>
-      <c r="F3" s="41"/>
-      <c r="G3" s="41"/>
-      <c r="H3" s="41"/>
-      <c r="I3" s="41"/>
-      <c r="J3" s="41"/>
-      <c r="K3" s="41"/>
-      <c r="L3" s="41"/>
-      <c r="M3" s="41"/>
+      <c r="B3" s="40"/>
+      <c r="C3" s="40"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="40"/>
+      <c r="H3" s="40"/>
+      <c r="I3" s="40"/>
+      <c r="J3" s="40"/>
+      <c r="K3" s="40"/>
+      <c r="L3" s="40"/>
+      <c r="M3" s="40"/>
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B4" s="41"/>
-      <c r="C4" s="41"/>
-      <c r="D4" s="41"/>
-      <c r="E4" s="41"/>
-      <c r="F4" s="41"/>
-      <c r="G4" s="41"/>
-      <c r="H4" s="41"/>
-      <c r="I4" s="41"/>
-      <c r="J4" s="41"/>
-      <c r="K4" s="41"/>
-      <c r="L4" s="41"/>
-      <c r="M4" s="41"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="40"/>
+      <c r="J4" s="40"/>
+      <c r="K4" s="40"/>
+      <c r="L4" s="40"/>
+      <c r="M4" s="40"/>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B5" s="41"/>
-      <c r="C5" s="41"/>
-      <c r="D5" s="41"/>
-      <c r="E5" s="41"/>
-      <c r="F5" s="41"/>
-      <c r="G5" s="41"/>
-      <c r="H5" s="41"/>
-      <c r="I5" s="41"/>
-      <c r="J5" s="41"/>
-      <c r="K5" s="41"/>
-      <c r="L5" s="41"/>
-      <c r="M5" s="41"/>
+      <c r="B5" s="40"/>
+      <c r="C5" s="40"/>
+      <c r="D5" s="40"/>
+      <c r="E5" s="40"/>
+      <c r="F5" s="40"/>
+      <c r="G5" s="40"/>
+      <c r="H5" s="40"/>
+      <c r="I5" s="40"/>
+      <c r="J5" s="40"/>
+      <c r="K5" s="40"/>
+      <c r="L5" s="40"/>
+      <c r="M5" s="40"/>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B6" s="41"/>
-      <c r="C6" s="41"/>
-      <c r="D6" s="41"/>
-      <c r="E6" s="41"/>
-      <c r="F6" s="41"/>
-      <c r="G6" s="41"/>
-      <c r="H6" s="41"/>
-      <c r="I6" s="41"/>
-      <c r="J6" s="41"/>
-      <c r="K6" s="41"/>
-      <c r="L6" s="41"/>
-      <c r="M6" s="41"/>
+      <c r="B6" s="40"/>
+      <c r="C6" s="40"/>
+      <c r="D6" s="40"/>
+      <c r="E6" s="40"/>
+      <c r="F6" s="40"/>
+      <c r="G6" s="40"/>
+      <c r="H6" s="40"/>
+      <c r="I6" s="40"/>
+      <c r="J6" s="40"/>
+      <c r="K6" s="40"/>
+      <c r="L6" s="40"/>
+      <c r="M6" s="40"/>
     </row>
     <row r="27" spans="2:11" x14ac:dyDescent="0.25">
       <c r="K27" s="38" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="31" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B31" s="38" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -1530,20 +1555,20 @@
   <dimension ref="A1:P11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" customWidth="1"/>
     <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.7109375" customWidth="1"/>
     <col min="6" max="6" width="25.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9.140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="28.85546875" bestFit="1" customWidth="1"/>
@@ -1579,8 +1604,8 @@
         <v>9</v>
       </c>
       <c r="B3" s="38"/>
-      <c r="C3" s="46" t="s">
-        <v>126</v>
+      <c r="C3" s="44" t="s">
+        <v>123</v>
       </c>
       <c r="D3" s="38"/>
       <c r="E3" s="38"/>
@@ -1595,103 +1620,91 @@
       <c r="A4" t="s">
         <v>106</v>
       </c>
-      <c r="B4" s="45" t="s">
-        <v>116</v>
-      </c>
-      <c r="C4" s="40" t="s">
+      <c r="B4" s="47" t="s">
+        <v>114</v>
+      </c>
+      <c r="C4" s="39" t="s">
         <v>107</v>
       </c>
       <c r="D4" s="31" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="E4" s="32" t="s">
         <v>109</v>
       </c>
-      <c r="F4" s="39">
-        <v>1</v>
-      </c>
-      <c r="G4" s="38"/>
-      <c r="H4" s="37" t="s">
+      <c r="F4" s="37" t="s">
         <v>107</v>
       </c>
-      <c r="I4" s="36" t="s">
-        <v>114</v>
-      </c>
-      <c r="J4" s="33" t="s">
+      <c r="G4" s="36" t="s">
+        <v>113</v>
+      </c>
+      <c r="H4" s="33" t="s">
         <v>108</v>
       </c>
-      <c r="K4" s="34" t="s">
-        <v>109</v>
+      <c r="I4" s="34" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B5" s="38" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C5" s="38"/>
       <c r="D5" s="38"/>
       <c r="E5" s="38"/>
-      <c r="F5" s="44">
-        <v>1</v>
-      </c>
+      <c r="F5" s="38"/>
       <c r="G5" s="38"/>
       <c r="H5" s="38"/>
       <c r="I5" s="38"/>
-      <c r="J5" s="38"/>
-      <c r="K5" s="38"/>
-      <c r="L5" s="1" t="s">
+      <c r="J5" s="1" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B8" s="45" t="s">
+      <c r="B8" s="43" t="s">
+        <v>124</v>
+      </c>
+      <c r="C8" s="46" t="s">
+        <v>125</v>
+      </c>
+      <c r="D8" s="45" t="s">
+        <v>126</v>
+      </c>
+      <c r="E8" s="45" t="s">
+        <v>127</v>
+      </c>
+      <c r="F8" s="38" t="s">
+        <v>119</v>
+      </c>
+      <c r="G8" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="C8" s="47" t="s">
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="E10" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="F11" s="35" t="s">
         <v>110</v>
       </c>
-      <c r="D8" s="47" t="s">
-        <v>124</v>
-      </c>
-      <c r="E8" s="47" t="s">
+      <c r="G11" s="35" t="s">
         <v>112</v>
       </c>
-      <c r="F8" s="38"/>
-      <c r="G8" s="38" t="s">
+      <c r="H11" s="35" t="s">
+        <v>111</v>
+      </c>
+      <c r="I11" s="35" t="s">
+        <v>129</v>
+      </c>
+      <c r="J11" s="1" t="s">
         <v>121</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="F10" s="1" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="G11" s="45" t="s">
-        <v>115</v>
-      </c>
-      <c r="H11" s="35" t="s">
-        <v>110</v>
-      </c>
-      <c r="I11" s="35" t="s">
-        <v>113</v>
-      </c>
-      <c r="J11" s="35" t="s">
-        <v>111</v>
-      </c>
-      <c r="K11" s="35" t="s">
-        <v>112</v>
-      </c>
-      <c r="L11" s="1" t="s">
-        <v>123</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Carry on Excel tests solution
</commit_message>
<xml_diff>
--- a/TestsAndDemos/Tests/Etk.Tests.Templates.ExcelDna1/Etk.Tests.Templates.ExcelDna1.xlsx
+++ b/TestsAndDemos/Tests/Etk.Tests.Templates.ExcelDna1/Etk.Tests.Templates.ExcelDna1.xlsx
@@ -371,9 +371,6 @@
     <t>Done</t>
   </si>
   <si>
-    <t>[Execute All Tests]</t>
-  </si>
-  <si>
     <t>&lt;EndTemplate Name='AllTests'/&gt;</t>
   </si>
   <si>
@@ -401,9 +398,6 @@
     <t>{?Search...?}</t>
   </si>
   <si>
-    <t>[ME=ExcelTests,Etk.Tests.Templates.ExcelDna1,GetNumberOfTests:Execute]</t>
-  </si>
-  <si>
     <t>{ME=ExcelTests,Etk.Tests.Templates.ExcelDna1,GetNumberOfTests:Description}</t>
   </si>
   <si>
@@ -417,6 +411,12 @@
   </si>
   <si>
     <t>{Errors}</t>
+  </si>
+  <si>
+    <t>[LDC=ExcelTestsManager,,Execute:Execute All Tests]</t>
+  </si>
+  <si>
+    <t>[ME=ExcelTests,,GetNumberOfTests;LDC=ExcelTests,,ExecuteAsync:Execute]</t>
   </si>
 </sst>
 </file>
@@ -1078,6 +1078,42 @@
     <xf numFmtId="49" fontId="0" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1100,24 +1136,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1131,24 +1149,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1532,12 +1532,12 @@
     </row>
     <row r="27" spans="2:11" x14ac:dyDescent="0.25">
       <c r="K27" s="38" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="31" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B31" s="38" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -1555,7 +1555,7 @@
   <dimension ref="A1:P11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1605,7 +1605,7 @@
       </c>
       <c r="B3" s="38"/>
       <c r="C3" s="44" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D3" s="38"/>
       <c r="E3" s="38"/>
@@ -1621,13 +1621,13 @@
         <v>106</v>
       </c>
       <c r="B4" s="47" t="s">
-        <v>114</v>
+        <v>128</v>
       </c>
       <c r="C4" s="39" t="s">
         <v>107</v>
       </c>
       <c r="D4" s="31" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E4" s="32" t="s">
         <v>109</v>
@@ -1642,12 +1642,12 @@
         <v>108</v>
       </c>
       <c r="I4" s="34" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B5" s="38" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C5" s="38"/>
       <c r="D5" s="38"/>
@@ -1662,32 +1662,32 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B8" s="43" t="s">
+        <v>129</v>
+      </c>
+      <c r="C8" s="46" t="s">
+        <v>123</v>
+      </c>
+      <c r="D8" s="45" t="s">
         <v>124</v>
       </c>
-      <c r="C8" s="46" t="s">
+      <c r="E8" s="45" t="s">
         <v>125</v>
       </c>
-      <c r="D8" s="45" t="s">
-        <v>126</v>
-      </c>
-      <c r="E8" s="45" t="s">
-        <v>127</v>
-      </c>
       <c r="F8" s="38" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="E10" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
@@ -1701,10 +1701,10 @@
         <v>111</v>
       </c>
       <c r="I11" s="35" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -2013,24 +2013,24 @@
       <c r="P1" s="50"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="74" t="s">
+      <c r="A2" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="75"/>
-      <c r="C2" s="75"/>
-      <c r="D2" s="75"/>
-      <c r="E2" s="75"/>
-      <c r="F2" s="75"/>
-      <c r="G2" s="75"/>
-      <c r="H2" s="75"/>
-      <c r="I2" s="75"/>
-      <c r="J2" s="75"/>
-      <c r="K2" s="75"/>
-      <c r="L2" s="75"/>
-      <c r="M2" s="75"/>
-      <c r="N2" s="75"/>
-      <c r="O2" s="75"/>
-      <c r="P2" s="76"/>
+      <c r="B2" s="64"/>
+      <c r="C2" s="64"/>
+      <c r="D2" s="64"/>
+      <c r="E2" s="64"/>
+      <c r="F2" s="64"/>
+      <c r="G2" s="64"/>
+      <c r="H2" s="64"/>
+      <c r="I2" s="64"/>
+      <c r="J2" s="64"/>
+      <c r="K2" s="64"/>
+      <c r="L2" s="64"/>
+      <c r="M2" s="64"/>
+      <c r="N2" s="64"/>
+      <c r="O2" s="64"/>
+      <c r="P2" s="65"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -2055,24 +2055,24 @@
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="74" t="s">
+      <c r="A6" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="75"/>
-      <c r="C6" s="75"/>
-      <c r="D6" s="75"/>
-      <c r="E6" s="75"/>
-      <c r="F6" s="75"/>
-      <c r="G6" s="75"/>
-      <c r="H6" s="75"/>
-      <c r="I6" s="75"/>
-      <c r="J6" s="75"/>
-      <c r="K6" s="75"/>
-      <c r="L6" s="75"/>
-      <c r="M6" s="75"/>
-      <c r="N6" s="75"/>
-      <c r="O6" s="75"/>
-      <c r="P6" s="76"/>
+      <c r="B6" s="64"/>
+      <c r="C6" s="64"/>
+      <c r="D6" s="64"/>
+      <c r="E6" s="64"/>
+      <c r="F6" s="64"/>
+      <c r="G6" s="64"/>
+      <c r="H6" s="64"/>
+      <c r="I6" s="64"/>
+      <c r="J6" s="64"/>
+      <c r="K6" s="64"/>
+      <c r="L6" s="64"/>
+      <c r="M6" s="64"/>
+      <c r="N6" s="64"/>
+      <c r="O6" s="64"/>
+      <c r="P6" s="65"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -2115,35 +2115,35 @@
       <c r="A10" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="81" t="s">
+      <c r="B10" s="66" t="s">
         <v>44</v>
       </c>
-      <c r="C10" s="82"/>
-      <c r="D10" s="82"/>
-      <c r="E10" s="83"/>
+      <c r="C10" s="67"/>
+      <c r="D10" s="67"/>
+      <c r="E10" s="68"/>
       <c r="F10" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" s="74" t="s">
+      <c r="A13" s="63" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="75"/>
-      <c r="C13" s="75"/>
-      <c r="D13" s="75"/>
-      <c r="E13" s="75"/>
-      <c r="F13" s="75"/>
-      <c r="G13" s="75"/>
-      <c r="H13" s="75"/>
-      <c r="I13" s="75"/>
-      <c r="J13" s="75"/>
-      <c r="K13" s="75"/>
-      <c r="L13" s="75"/>
-      <c r="M13" s="75"/>
-      <c r="N13" s="75"/>
-      <c r="O13" s="75"/>
-      <c r="P13" s="76"/>
+      <c r="B13" s="64"/>
+      <c r="C13" s="64"/>
+      <c r="D13" s="64"/>
+      <c r="E13" s="64"/>
+      <c r="F13" s="64"/>
+      <c r="G13" s="64"/>
+      <c r="H13" s="64"/>
+      <c r="I13" s="64"/>
+      <c r="J13" s="64"/>
+      <c r="K13" s="64"/>
+      <c r="L13" s="64"/>
+      <c r="M13" s="64"/>
+      <c r="N13" s="64"/>
+      <c r="O13" s="64"/>
+      <c r="P13" s="65"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
@@ -2154,12 +2154,12 @@
       <c r="A15" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="81" t="s">
+      <c r="B15" s="66" t="s">
         <v>44</v>
       </c>
-      <c r="C15" s="82"/>
-      <c r="D15" s="82"/>
-      <c r="E15" s="83"/>
+      <c r="C15" s="67"/>
+      <c r="D15" s="67"/>
+      <c r="E15" s="68"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
@@ -2197,23 +2197,23 @@
       <c r="A18" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B18" s="81" t="s">
+      <c r="B18" s="66" t="s">
         <v>45</v>
       </c>
-      <c r="C18" s="82"/>
-      <c r="D18" s="82"/>
-      <c r="E18" s="83"/>
+      <c r="C18" s="67"/>
+      <c r="D18" s="67"/>
+      <c r="E18" s="68"/>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="81" t="s">
+      <c r="B19" s="66" t="s">
         <v>44</v>
       </c>
-      <c r="C19" s="82"/>
-      <c r="D19" s="82"/>
-      <c r="E19" s="83"/>
+      <c r="C19" s="67"/>
+      <c r="D19" s="67"/>
+      <c r="E19" s="68"/>
       <c r="F19" s="1" t="s">
         <v>8</v>
       </c>
@@ -2239,24 +2239,24 @@
       <c r="P23" s="50"/>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A24" s="74" t="s">
+      <c r="A24" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="B24" s="75"/>
-      <c r="C24" s="75"/>
-      <c r="D24" s="75"/>
-      <c r="E24" s="75"/>
-      <c r="F24" s="75"/>
-      <c r="G24" s="75"/>
-      <c r="H24" s="75"/>
-      <c r="I24" s="75"/>
-      <c r="J24" s="75"/>
-      <c r="K24" s="75"/>
-      <c r="L24" s="75"/>
-      <c r="M24" s="75"/>
-      <c r="N24" s="75"/>
-      <c r="O24" s="75"/>
-      <c r="P24" s="76"/>
+      <c r="B24" s="64"/>
+      <c r="C24" s="64"/>
+      <c r="D24" s="64"/>
+      <c r="E24" s="64"/>
+      <c r="F24" s="64"/>
+      <c r="G24" s="64"/>
+      <c r="H24" s="64"/>
+      <c r="I24" s="64"/>
+      <c r="J24" s="64"/>
+      <c r="K24" s="64"/>
+      <c r="L24" s="64"/>
+      <c r="M24" s="64"/>
+      <c r="N24" s="64"/>
+      <c r="O24" s="64"/>
+      <c r="P24" s="65"/>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
@@ -2300,24 +2300,24 @@
       <c r="A32" s="1"/>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A35" s="74" t="s">
+      <c r="A35" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="B35" s="75"/>
-      <c r="C35" s="75"/>
-      <c r="D35" s="75"/>
-      <c r="E35" s="75"/>
-      <c r="F35" s="75"/>
-      <c r="G35" s="75"/>
-      <c r="H35" s="75"/>
-      <c r="I35" s="75"/>
-      <c r="J35" s="75"/>
-      <c r="K35" s="75"/>
-      <c r="L35" s="75"/>
-      <c r="M35" s="75"/>
-      <c r="N35" s="75"/>
-      <c r="O35" s="75"/>
-      <c r="P35" s="76"/>
+      <c r="B35" s="64"/>
+      <c r="C35" s="64"/>
+      <c r="D35" s="64"/>
+      <c r="E35" s="64"/>
+      <c r="F35" s="64"/>
+      <c r="G35" s="64"/>
+      <c r="H35" s="64"/>
+      <c r="I35" s="64"/>
+      <c r="J35" s="64"/>
+      <c r="K35" s="64"/>
+      <c r="L35" s="64"/>
+      <c r="M35" s="64"/>
+      <c r="N35" s="64"/>
+      <c r="O35" s="64"/>
+      <c r="P35" s="65"/>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
@@ -2338,7 +2338,7 @@
       <c r="C37" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="D37" s="84" t="s">
+      <c r="D37" s="72" t="s">
         <v>46</v>
       </c>
     </row>
@@ -2350,7 +2350,7 @@
       <c r="C38" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="D38" s="85"/>
+      <c r="D38" s="73"/>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
@@ -2360,7 +2360,7 @@
       <c r="C39" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D39" s="85"/>
+      <c r="D39" s="73"/>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
@@ -2370,30 +2370,30 @@
       <c r="C40" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="D40" s="86"/>
+      <c r="D40" s="74"/>
       <c r="E40" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A44" s="74" t="s">
+      <c r="A44" s="63" t="s">
         <v>7</v>
       </c>
-      <c r="B44" s="75"/>
-      <c r="C44" s="75"/>
-      <c r="D44" s="75"/>
-      <c r="E44" s="75"/>
-      <c r="F44" s="75"/>
-      <c r="G44" s="75"/>
-      <c r="H44" s="75"/>
-      <c r="I44" s="75"/>
-      <c r="J44" s="75"/>
-      <c r="K44" s="75"/>
-      <c r="L44" s="75"/>
-      <c r="M44" s="75"/>
-      <c r="N44" s="75"/>
-      <c r="O44" s="75"/>
-      <c r="P44" s="76"/>
+      <c r="B44" s="64"/>
+      <c r="C44" s="64"/>
+      <c r="D44" s="64"/>
+      <c r="E44" s="64"/>
+      <c r="F44" s="64"/>
+      <c r="G44" s="64"/>
+      <c r="H44" s="64"/>
+      <c r="I44" s="64"/>
+      <c r="J44" s="64"/>
+      <c r="K44" s="64"/>
+      <c r="L44" s="64"/>
+      <c r="M44" s="64"/>
+      <c r="N44" s="64"/>
+      <c r="O44" s="64"/>
+      <c r="P44" s="65"/>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
@@ -2413,7 +2413,7 @@
       </c>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B46" s="71" t="s">
+      <c r="B46" s="69" t="s">
         <v>46</v>
       </c>
       <c r="C46" s="3" t="s">
@@ -2422,45 +2422,45 @@
       <c r="D46" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="E46" s="71" t="s">
+      <c r="E46" s="69" t="s">
         <v>45</v>
       </c>
-      <c r="F46" s="84" t="s">
+      <c r="F46" s="72" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B47" s="72"/>
+      <c r="B47" s="70"/>
       <c r="C47" s="3" t="s">
         <v>41</v>
       </c>
       <c r="D47" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="E47" s="72"/>
-      <c r="F47" s="85"/>
+      <c r="E47" s="70"/>
+      <c r="F47" s="73"/>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B48" s="72"/>
+      <c r="B48" s="70"/>
       <c r="C48" s="3" t="s">
         <v>42</v>
       </c>
       <c r="D48" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="E48" s="72"/>
-      <c r="F48" s="85"/>
+      <c r="E48" s="70"/>
+      <c r="F48" s="73"/>
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B49" s="73"/>
+      <c r="B49" s="71"/>
       <c r="C49" s="3" t="s">
         <v>43</v>
       </c>
       <c r="D49" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="E49" s="73"/>
-      <c r="F49" s="86"/>
+      <c r="E49" s="71"/>
+      <c r="F49" s="74"/>
       <c r="G49" s="1" t="s">
         <v>16</v>
       </c>
@@ -2486,35 +2486,35 @@
       <c r="P56" s="50"/>
     </row>
     <row r="57" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A57" s="74" t="s">
+      <c r="A57" s="63" t="s">
         <v>85</v>
       </c>
-      <c r="B57" s="75"/>
-      <c r="C57" s="75"/>
-      <c r="D57" s="75"/>
-      <c r="E57" s="75"/>
-      <c r="F57" s="75"/>
-      <c r="G57" s="75"/>
-      <c r="H57" s="75"/>
-      <c r="I57" s="75"/>
-      <c r="J57" s="75"/>
-      <c r="K57" s="75"/>
-      <c r="L57" s="75"/>
-      <c r="M57" s="75"/>
-      <c r="N57" s="75"/>
-      <c r="O57" s="75"/>
-      <c r="P57" s="76"/>
+      <c r="B57" s="64"/>
+      <c r="C57" s="64"/>
+      <c r="D57" s="64"/>
+      <c r="E57" s="64"/>
+      <c r="F57" s="64"/>
+      <c r="G57" s="64"/>
+      <c r="H57" s="64"/>
+      <c r="I57" s="64"/>
+      <c r="J57" s="64"/>
+      <c r="K57" s="64"/>
+      <c r="L57" s="64"/>
+      <c r="M57" s="64"/>
+      <c r="N57" s="64"/>
+      <c r="O57" s="64"/>
+      <c r="P57" s="65"/>
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B59" s="81" t="s">
+      <c r="B59" s="66" t="s">
         <v>46</v>
       </c>
-      <c r="C59" s="82"/>
-      <c r="D59" s="82"/>
-      <c r="E59" s="83"/>
+      <c r="C59" s="67"/>
+      <c r="D59" s="67"/>
+      <c r="E59" s="68"/>
       <c r="F59" s="16"/>
       <c r="G59" s="16"/>
       <c r="H59" s="16"/>
@@ -2573,13 +2573,13 @@
       <c r="N61" s="16"/>
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B62" s="80" t="s">
+      <c r="B62" s="86" t="s">
         <v>102</v>
       </c>
-      <c r="C62" s="80"/>
-      <c r="D62" s="80"/>
-      <c r="E62" s="80"/>
-      <c r="F62" s="80"/>
+      <c r="C62" s="86"/>
+      <c r="D62" s="86"/>
+      <c r="E62" s="86"/>
+      <c r="F62" s="86"/>
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B63" s="5" t="s">
@@ -2618,16 +2618,16 @@
       <c r="F66" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="G66" s="77" t="s">
+      <c r="G66" s="83" t="s">
         <v>50</v>
       </c>
-      <c r="H66" s="78"/>
-      <c r="I66" s="78"/>
-      <c r="J66" s="78"/>
-      <c r="K66" s="78"/>
-      <c r="L66" s="78"/>
-      <c r="M66" s="78"/>
-      <c r="N66" s="79"/>
+      <c r="H66" s="84"/>
+      <c r="I66" s="84"/>
+      <c r="J66" s="84"/>
+      <c r="K66" s="84"/>
+      <c r="L66" s="84"/>
+      <c r="M66" s="84"/>
+      <c r="N66" s="85"/>
       <c r="O66" s="16"/>
       <c r="P66" s="16"/>
       <c r="Q66" s="16"/>
@@ -2821,24 +2821,24 @@
       </c>
     </row>
     <row r="81" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A81" s="74" t="s">
+      <c r="A81" s="63" t="s">
         <v>99</v>
       </c>
-      <c r="B81" s="75"/>
-      <c r="C81" s="75"/>
-      <c r="D81" s="75"/>
-      <c r="E81" s="75"/>
-      <c r="F81" s="75"/>
-      <c r="G81" s="75"/>
-      <c r="H81" s="75"/>
-      <c r="I81" s="75"/>
-      <c r="J81" s="75"/>
-      <c r="K81" s="75"/>
-      <c r="L81" s="75"/>
-      <c r="M81" s="75"/>
-      <c r="N81" s="75"/>
-      <c r="O81" s="75"/>
-      <c r="P81" s="76"/>
+      <c r="B81" s="64"/>
+      <c r="C81" s="64"/>
+      <c r="D81" s="64"/>
+      <c r="E81" s="64"/>
+      <c r="F81" s="64"/>
+      <c r="G81" s="64"/>
+      <c r="H81" s="64"/>
+      <c r="I81" s="64"/>
+      <c r="J81" s="64"/>
+      <c r="K81" s="64"/>
+      <c r="L81" s="64"/>
+      <c r="M81" s="64"/>
+      <c r="N81" s="64"/>
+      <c r="O81" s="64"/>
+      <c r="P81" s="65"/>
     </row>
     <row r="83" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
@@ -2853,7 +2853,7 @@
     </row>
     <row r="84" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A84" s="1"/>
-      <c r="B84" s="71" t="s">
+      <c r="B84" s="69" t="s">
         <v>46</v>
       </c>
       <c r="C84" s="3" t="s">
@@ -2868,7 +2868,7 @@
     </row>
     <row r="85" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A85" s="1"/>
-      <c r="B85" s="72"/>
+      <c r="B85" s="70"/>
       <c r="C85" s="3" t="s">
         <v>41</v>
       </c>
@@ -2878,7 +2878,7 @@
     </row>
     <row r="86" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A86" s="1"/>
-      <c r="B86" s="72"/>
+      <c r="B86" s="70"/>
       <c r="C86" s="3" t="s">
         <v>42</v>
       </c>
@@ -2887,7 +2887,7 @@
       </c>
     </row>
     <row r="87" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B87" s="73"/>
+      <c r="B87" s="71"/>
       <c r="C87" s="3" t="s">
         <v>43</v>
       </c>
@@ -2917,7 +2917,7 @@
       <c r="L90" s="17"/>
     </row>
     <row r="91" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B91" s="63" t="s">
+      <c r="B91" s="75" t="s">
         <v>49</v>
       </c>
       <c r="C91" s="23" t="s">
@@ -2931,7 +2931,7 @@
       </c>
     </row>
     <row r="92" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B92" s="64"/>
+      <c r="B92" s="76"/>
       <c r="C92" s="23" t="s">
         <v>52</v>
       </c>
@@ -2941,7 +2941,7 @@
       <c r="E92" s="16"/>
     </row>
     <row r="93" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B93" s="64"/>
+      <c r="B93" s="76"/>
       <c r="C93" s="23" t="s">
         <v>53</v>
       </c>
@@ -2952,7 +2952,7 @@
       <c r="F93" s="16"/>
     </row>
     <row r="94" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B94" s="64"/>
+      <c r="B94" s="76"/>
       <c r="C94" s="23" t="s">
         <v>41</v>
       </c>
@@ -2963,7 +2963,7 @@
       <c r="F94" s="16"/>
     </row>
     <row r="95" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B95" s="65"/>
+      <c r="B95" s="77"/>
       <c r="C95" s="24" t="s">
         <v>42</v>
       </c>
@@ -2987,7 +2987,7 @@
       </c>
     </row>
     <row r="99" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B99" s="66" t="s">
+      <c r="B99" s="78" t="s">
         <v>50</v>
       </c>
       <c r="C99" s="25" t="s">
@@ -3001,7 +3001,7 @@
       </c>
     </row>
     <row r="100" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B100" s="67"/>
+      <c r="B100" s="79"/>
       <c r="C100" s="25" t="s">
         <v>58</v>
       </c>
@@ -3046,7 +3046,7 @@
     </row>
     <row r="106" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A106" s="5"/>
-      <c r="B106" s="68" t="s">
+      <c r="B106" s="80" t="s">
         <v>54</v>
       </c>
       <c r="C106" s="7" t="s">
@@ -3059,7 +3059,7 @@
       <c r="J106" s="5"/>
     </row>
     <row r="107" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B107" s="69"/>
+      <c r="B107" s="81"/>
       <c r="C107" s="7" t="s">
         <v>75</v>
       </c>
@@ -3068,7 +3068,7 @@
       </c>
     </row>
     <row r="108" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B108" s="69"/>
+      <c r="B108" s="81"/>
       <c r="C108" s="7" t="s">
         <v>60</v>
       </c>
@@ -3077,7 +3077,7 @@
       </c>
     </row>
     <row r="109" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B109" s="69"/>
+      <c r="B109" s="81"/>
       <c r="C109" s="7" t="s">
         <v>61</v>
       </c>
@@ -3086,7 +3086,7 @@
       </c>
     </row>
     <row r="110" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B110" s="69"/>
+      <c r="B110" s="81"/>
       <c r="C110" s="7" t="s">
         <v>62</v>
       </c>
@@ -3095,7 +3095,7 @@
       </c>
     </row>
     <row r="111" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B111" s="70"/>
+      <c r="B111" s="82"/>
       <c r="C111" s="8" t="s">
         <v>63</v>
       </c>
@@ -3108,14 +3108,14 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="A35:P35"/>
-    <mergeCell ref="A44:P44"/>
-    <mergeCell ref="A57:P57"/>
-    <mergeCell ref="B59:E59"/>
-    <mergeCell ref="A56:P56"/>
-    <mergeCell ref="E46:E49"/>
-    <mergeCell ref="F46:F49"/>
-    <mergeCell ref="D37:D40"/>
+    <mergeCell ref="B91:B95"/>
+    <mergeCell ref="B99:B100"/>
+    <mergeCell ref="B106:B111"/>
+    <mergeCell ref="B46:B49"/>
+    <mergeCell ref="A81:P81"/>
+    <mergeCell ref="G66:N66"/>
+    <mergeCell ref="B84:B87"/>
+    <mergeCell ref="B62:F62"/>
     <mergeCell ref="A24:P24"/>
     <mergeCell ref="A1:P1"/>
     <mergeCell ref="A2:P2"/>
@@ -3126,14 +3126,14 @@
     <mergeCell ref="B10:E10"/>
     <mergeCell ref="B18:E18"/>
     <mergeCell ref="B19:E19"/>
-    <mergeCell ref="B91:B95"/>
-    <mergeCell ref="B99:B100"/>
-    <mergeCell ref="B106:B111"/>
-    <mergeCell ref="B46:B49"/>
-    <mergeCell ref="A81:P81"/>
-    <mergeCell ref="G66:N66"/>
-    <mergeCell ref="B84:B87"/>
-    <mergeCell ref="B62:F62"/>
+    <mergeCell ref="A35:P35"/>
+    <mergeCell ref="A44:P44"/>
+    <mergeCell ref="A57:P57"/>
+    <mergeCell ref="B59:E59"/>
+    <mergeCell ref="A56:P56"/>
+    <mergeCell ref="E46:E49"/>
+    <mergeCell ref="F46:F49"/>
+    <mergeCell ref="D37:D40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Tests + few modifications on the search feature
</commit_message>
<xml_diff>
--- a/TestsAndDemos/Tests/Etk.Tests.Templates.ExcelDna1/Etk.Tests.Templates.ExcelDna1.xlsx
+++ b/TestsAndDemos/Tests/Etk.Tests.Templates.ExcelDna1/Etk.Tests.Templates.ExcelDna1.xlsx
@@ -31,6 +31,43 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>BlouinSide</author>
+  </authors>
+  <commentList>
+    <comment ref="C8" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Double left clic to filter the view on this test topic.
+Double left clic again to remove the filter.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F11" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Double left clic to display the sheet we are testing.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="116">
   <si>
@@ -298,9 +335,6 @@
     <t>Exception</t>
   </si>
   <si>
-    <t>{Description}</t>
-  </si>
-  <si>
     <t>Done</t>
   </si>
   <si>
@@ -337,9 +371,6 @@
     <t>&lt;EndTemplate Name='TestTopics'/&gt;</t>
   </si>
   <si>
-    <t>{ME=ExcelTestTopic,,GetNumberOfTests:Description}</t>
-  </si>
-  <si>
     <t>[ME=ExcelTestTopic,,GetNumberOfTests;LDC=ExcelTestTopic,,Execute:Execute]</t>
   </si>
   <si>
@@ -380,13 +411,19 @@
   </si>
   <si>
     <t>&lt;Template Name='TestTopics' BindingWith='IExcelTestTopic'/&gt;</t>
+  </si>
+  <si>
+    <t>{ME=ExcelTestTopic,,GetNumberOfTests;LDC=ExcelTestsManager,Etk.Tests.Templates.ExcelDna1,SetSearchValue:Description}</t>
+  </si>
+  <si>
+    <t>{LDC=ExcelTest,Etk.Tests.Templates.ExcelDna1,DisplayResultSheet:Description}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -436,6 +473,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="27">
@@ -1032,24 +1075,6 @@
     <xf numFmtId="49" fontId="0" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1061,6 +1086,24 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1444,12 +1487,12 @@
     </row>
     <row r="27" spans="2:11" x14ac:dyDescent="0.25">
       <c r="K27" s="32" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="31" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B31" s="32" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -1460,14 +1503,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="4" tint="0.39997558519241921"/>
   </sheetPr>
   <dimension ref="A1:P19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1508,7 +1551,7 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1516,10 +1559,10 @@
         <v>9</v>
       </c>
       <c r="B3" s="43" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C3" s="38" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D3" s="32"/>
       <c r="E3" s="32"/>
@@ -1535,13 +1578,13 @@
         <v>84</v>
       </c>
       <c r="B4" s="41" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C4" s="33" t="s">
         <v>85</v>
       </c>
       <c r="D4" s="25" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E4" s="26" t="s">
         <v>87</v>
@@ -1550,18 +1593,18 @@
         <v>85</v>
       </c>
       <c r="G4" s="30" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H4" s="27" t="s">
         <v>86</v>
       </c>
       <c r="I4" s="28" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B5" s="32" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C5" s="32"/>
       <c r="D5" s="32"/>
@@ -1576,54 +1619,54 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B8" s="37" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C8" s="40" t="s">
+        <v>114</v>
+      </c>
+      <c r="D8" s="39" t="s">
+        <v>109</v>
+      </c>
+      <c r="E8" s="39" t="s">
         <v>101</v>
       </c>
-      <c r="D8" s="39" t="s">
-        <v>111</v>
-      </c>
-      <c r="E8" s="39" t="s">
-        <v>103</v>
-      </c>
       <c r="F8" s="32" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="E10" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="F11" s="29" t="s">
-        <v>88</v>
+        <v>115</v>
       </c>
       <c r="G11" s="29" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="H11" s="29" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="I11" s="29" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="16" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="49" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B16" s="50"/>
       <c r="C16" s="50"/>
@@ -1631,44 +1674,44 @@
     </row>
     <row r="17" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="42" t="s">
+        <v>103</v>
+      </c>
+      <c r="B17" s="42" t="s">
         <v>105</v>
       </c>
-      <c r="B17" s="42" t="s">
+      <c r="C17" s="42" t="s">
         <v>107</v>
       </c>
-      <c r="C17" s="42" t="s">
-        <v>109</v>
-      </c>
       <c r="D17" s="42" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="43" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B18" s="39" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C18" s="29" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D18" s="29" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="44" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B19" s="45" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C19" s="45" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D19" s="45" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -1678,6 +1721,7 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1978,24 +2022,24 @@
       <c r="P1" s="48"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="63" t="s">
+      <c r="A2" s="67" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="64"/>
-      <c r="C2" s="64"/>
-      <c r="D2" s="64"/>
-      <c r="E2" s="64"/>
-      <c r="F2" s="64"/>
-      <c r="G2" s="64"/>
-      <c r="H2" s="64"/>
-      <c r="I2" s="64"/>
-      <c r="J2" s="64"/>
-      <c r="K2" s="64"/>
-      <c r="L2" s="64"/>
-      <c r="M2" s="64"/>
-      <c r="N2" s="64"/>
-      <c r="O2" s="64"/>
-      <c r="P2" s="65"/>
+      <c r="B2" s="68"/>
+      <c r="C2" s="68"/>
+      <c r="D2" s="68"/>
+      <c r="E2" s="68"/>
+      <c r="F2" s="68"/>
+      <c r="G2" s="68"/>
+      <c r="H2" s="68"/>
+      <c r="I2" s="68"/>
+      <c r="J2" s="68"/>
+      <c r="K2" s="68"/>
+      <c r="L2" s="68"/>
+      <c r="M2" s="68"/>
+      <c r="N2" s="68"/>
+      <c r="O2" s="68"/>
+      <c r="P2" s="69"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -2020,24 +2064,24 @@
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="63" t="s">
+      <c r="A6" s="67" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="64"/>
-      <c r="C6" s="64"/>
-      <c r="D6" s="64"/>
-      <c r="E6" s="64"/>
-      <c r="F6" s="64"/>
-      <c r="G6" s="64"/>
-      <c r="H6" s="64"/>
-      <c r="I6" s="64"/>
-      <c r="J6" s="64"/>
-      <c r="K6" s="64"/>
-      <c r="L6" s="64"/>
-      <c r="M6" s="64"/>
-      <c r="N6" s="64"/>
-      <c r="O6" s="64"/>
-      <c r="P6" s="65"/>
+      <c r="B6" s="68"/>
+      <c r="C6" s="68"/>
+      <c r="D6" s="68"/>
+      <c r="E6" s="68"/>
+      <c r="F6" s="68"/>
+      <c r="G6" s="68"/>
+      <c r="H6" s="68"/>
+      <c r="I6" s="68"/>
+      <c r="J6" s="68"/>
+      <c r="K6" s="68"/>
+      <c r="L6" s="68"/>
+      <c r="M6" s="68"/>
+      <c r="N6" s="68"/>
+      <c r="O6" s="68"/>
+      <c r="P6" s="69"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -2080,35 +2124,35 @@
       <c r="A10" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="66" t="s">
+      <c r="B10" s="70" t="s">
         <v>37</v>
       </c>
-      <c r="C10" s="67"/>
-      <c r="D10" s="67"/>
-      <c r="E10" s="68"/>
+      <c r="C10" s="71"/>
+      <c r="D10" s="71"/>
+      <c r="E10" s="72"/>
       <c r="F10" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" s="63" t="s">
+      <c r="A13" s="67" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="64"/>
-      <c r="C13" s="64"/>
-      <c r="D13" s="64"/>
-      <c r="E13" s="64"/>
-      <c r="F13" s="64"/>
-      <c r="G13" s="64"/>
-      <c r="H13" s="64"/>
-      <c r="I13" s="64"/>
-      <c r="J13" s="64"/>
-      <c r="K13" s="64"/>
-      <c r="L13" s="64"/>
-      <c r="M13" s="64"/>
-      <c r="N13" s="64"/>
-      <c r="O13" s="64"/>
-      <c r="P13" s="65"/>
+      <c r="B13" s="68"/>
+      <c r="C13" s="68"/>
+      <c r="D13" s="68"/>
+      <c r="E13" s="68"/>
+      <c r="F13" s="68"/>
+      <c r="G13" s="68"/>
+      <c r="H13" s="68"/>
+      <c r="I13" s="68"/>
+      <c r="J13" s="68"/>
+      <c r="K13" s="68"/>
+      <c r="L13" s="68"/>
+      <c r="M13" s="68"/>
+      <c r="N13" s="68"/>
+      <c r="O13" s="68"/>
+      <c r="P13" s="69"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
@@ -2119,12 +2163,12 @@
       <c r="A15" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="66" t="s">
+      <c r="B15" s="70" t="s">
         <v>37</v>
       </c>
-      <c r="C15" s="67"/>
-      <c r="D15" s="67"/>
-      <c r="E15" s="68"/>
+      <c r="C15" s="71"/>
+      <c r="D15" s="71"/>
+      <c r="E15" s="72"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
@@ -2162,23 +2206,23 @@
       <c r="A18" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B18" s="66" t="s">
+      <c r="B18" s="70" t="s">
         <v>38</v>
       </c>
-      <c r="C18" s="67"/>
-      <c r="D18" s="67"/>
-      <c r="E18" s="68"/>
+      <c r="C18" s="71"/>
+      <c r="D18" s="71"/>
+      <c r="E18" s="72"/>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="66" t="s">
+      <c r="B19" s="70" t="s">
         <v>37</v>
       </c>
-      <c r="C19" s="67"/>
-      <c r="D19" s="67"/>
-      <c r="E19" s="68"/>
+      <c r="C19" s="71"/>
+      <c r="D19" s="71"/>
+      <c r="E19" s="72"/>
       <c r="F19" s="1" t="s">
         <v>8</v>
       </c>
@@ -2204,35 +2248,35 @@
       <c r="P24" s="48"/>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A25" s="63" t="s">
+      <c r="A25" s="67" t="s">
         <v>77</v>
       </c>
-      <c r="B25" s="64"/>
-      <c r="C25" s="64"/>
-      <c r="D25" s="64"/>
-      <c r="E25" s="64"/>
-      <c r="F25" s="64"/>
-      <c r="G25" s="64"/>
-      <c r="H25" s="64"/>
-      <c r="I25" s="64"/>
-      <c r="J25" s="64"/>
-      <c r="K25" s="64"/>
-      <c r="L25" s="64"/>
-      <c r="M25" s="64"/>
-      <c r="N25" s="64"/>
-      <c r="O25" s="64"/>
-      <c r="P25" s="65"/>
+      <c r="B25" s="68"/>
+      <c r="C25" s="68"/>
+      <c r="D25" s="68"/>
+      <c r="E25" s="68"/>
+      <c r="F25" s="68"/>
+      <c r="G25" s="68"/>
+      <c r="H25" s="68"/>
+      <c r="I25" s="68"/>
+      <c r="J25" s="68"/>
+      <c r="K25" s="68"/>
+      <c r="L25" s="68"/>
+      <c r="M25" s="68"/>
+      <c r="N25" s="68"/>
+      <c r="O25" s="68"/>
+      <c r="P25" s="69"/>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B27" s="66" t="s">
+      <c r="B27" s="70" t="s">
         <v>39</v>
       </c>
-      <c r="C27" s="67"/>
-      <c r="D27" s="67"/>
-      <c r="E27" s="68"/>
+      <c r="C27" s="71"/>
+      <c r="D27" s="71"/>
+      <c r="E27" s="72"/>
       <c r="F27" s="15"/>
       <c r="G27" s="15"/>
       <c r="H27" s="15"/>
@@ -2291,13 +2335,13 @@
       <c r="N29" s="15"/>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B30" s="72" t="s">
+      <c r="B30" s="66" t="s">
         <v>81</v>
       </c>
-      <c r="C30" s="72"/>
-      <c r="D30" s="72"/>
-      <c r="E30" s="72"/>
-      <c r="F30" s="72"/>
+      <c r="C30" s="66"/>
+      <c r="D30" s="66"/>
+      <c r="E30" s="66"/>
+      <c r="F30" s="66"/>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B31" s="4" t="s">
@@ -2336,16 +2380,16 @@
       <c r="F34" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="G34" s="69" t="s">
+      <c r="G34" s="63" t="s">
         <v>43</v>
       </c>
-      <c r="H34" s="70"/>
-      <c r="I34" s="70"/>
-      <c r="J34" s="70"/>
-      <c r="K34" s="70"/>
-      <c r="L34" s="70"/>
-      <c r="M34" s="70"/>
-      <c r="N34" s="71"/>
+      <c r="H34" s="64"/>
+      <c r="I34" s="64"/>
+      <c r="J34" s="64"/>
+      <c r="K34" s="64"/>
+      <c r="L34" s="64"/>
+      <c r="M34" s="64"/>
+      <c r="N34" s="65"/>
       <c r="O34" s="15"/>
       <c r="P34" s="15"/>
       <c r="Q34" s="15"/>

</xml_diff>

<commit_message>
Few bugs and improvements done
</commit_message>
<xml_diff>
--- a/TestsAndDemos/Tests/Etk.Tests.Templates.ExcelDna1/Etk.Tests.Templates.ExcelDna1.xlsx
+++ b/TestsAndDemos/Tests/Etk.Tests.Templates.ExcelDna1/Etk.Tests.Templates.ExcelDna1.xlsx
@@ -16,20 +16,11 @@
     <sheet name="Dashboard Templates" sheetId="5" r:id="rId2"/>
     <sheet name="BadTemplates" sheetId="3" r:id="rId3"/>
     <sheet name="BasicTemplates1" sheetId="1" r:id="rId4"/>
-    <sheet name="BasicEtkFeatures" sheetId="6" r:id="rId5"/>
-    <sheet name="VerticalMonoHeaderAndFooter" sheetId="7" r:id="rId6"/>
-    <sheet name="VerticalMultiHeaderAndFooter" sheetId="9" r:id="rId7"/>
-    <sheet name="VerticalNoHeaderAndFooter" sheetId="10" r:id="rId8"/>
-    <sheet name="VerticalWithOnlyOneLink" sheetId="11" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName name="DEC_DONE">'Dashboard Templates'!$C$20:$C$21</definedName>
     <definedName name="DEC_EXEC">'Dashboard Templates'!$D$20:$D$21</definedName>
     <definedName name="DEC_STATUS">'Dashboard Templates'!$A$20:$A$21</definedName>
-    <definedName name="Vertt_0" localSheetId="6">VerticalMultiHeaderAndFooter!$B$5</definedName>
-    <definedName name="Vertt_1" localSheetId="6">VerticalMultiHeaderAndFooter!$B$6</definedName>
-    <definedName name="Vertt_2" localSheetId="6">VerticalMultiHeaderAndFooter!$B$7</definedName>
-    <definedName name="Vertt_3" localSheetId="6">VerticalMultiHeaderAndFooter!$B$8</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
   <extLst>
@@ -46,6 +37,54 @@
     <author>BlouinSide</author>
   </authors>
   <commentList>
+    <comment ref="B6" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Double left click to execute all tests</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B10" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Double left click to execute the concerned tests</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="C10" authorId="0" shapeId="0">
       <text>
         <r>
@@ -60,7 +99,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F13" authorId="0" shapeId="0">
+    <comment ref="E13" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -73,6 +112,30 @@
         </r>
       </text>
     </comment>
+    <comment ref="B28" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Double left click to go back to the dashboard</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -326,9 +389,6 @@
     <t>Success</t>
   </si>
   <si>
-    <t>Exception</t>
-  </si>
-  <si>
     <t>Done</t>
   </si>
   <si>
@@ -341,122 +401,125 @@
     <t>&lt;EndTemplate Name='Tests'/&gt;</t>
   </si>
   <si>
+    <t>{?Search...?}</t>
+  </si>
+  <si>
+    <t>[LDC=ExcelTestsManager,,Execute:Execute All Tests]</t>
+  </si>
+  <si>
+    <t>&lt;Link To='TestTopics' With='TestTopics' /&gt;</t>
+  </si>
+  <si>
+    <t>&lt;EndTemplate Name='TestTopics'/&gt;</t>
+  </si>
+  <si>
+    <t>[ME=ExcelTestTopic,,GetNumberOfTests;LDC=ExcelTestTopic,,Execute:Execute]</t>
+  </si>
+  <si>
+    <t>Definition of the Decorators</t>
+  </si>
+  <si>
+    <t>DEC_STATUS</t>
+  </si>
+  <si>
+    <t>Text</t>
+  </si>
+  <si>
+    <t>DEC_INIT</t>
+  </si>
+  <si>
+    <t>DEC_EXEC</t>
+  </si>
+  <si>
+    <t>DEC_DONE</t>
+  </si>
+  <si>
+    <t>{DEC=DEC_STATUS:Status}</t>
+  </si>
+  <si>
+    <t>{DEC=DEC_DONE:Done}</t>
+  </si>
+  <si>
+    <t>{DEC=DEC_EXEC:Success}</t>
+  </si>
+  <si>
+    <t>&lt;Template Name='Main' BindingWith='ExcelTestsManager'/&gt;</t>
+  </si>
+  <si>
+    <t>{ME=ExcelTestTopic,,GetNumberOfTests;LDC=ExcelTestsManager,Etk.Tests.Templates.ExcelDna1,SetSearchValue:Description}</t>
+  </si>
+  <si>
+    <t>{LDC=ExcelTest,Etk.Tests.Templates.ExcelDna1,DisplayResultSheet:Description}</t>
+  </si>
+  <si>
+    <t>&lt;Template Name='TestTopics' BindingWith='IExcelTestTopic' /&gt;</t>
+  </si>
+  <si>
+    <t>Basic vertical templates (without linked templates)</t>
+  </si>
+  <si>
+    <t>Vertical templates with linked templates</t>
+  </si>
+  <si>
+    <t>Template with only a linked template</t>
+  </si>
+  <si>
+    <t>&lt;Link To='Products' With='GetAllProducts' /&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Template Name='Products' BindingWith='Product' /&gt;</t>
+  </si>
+  <si>
+    <t>{R:Name}</t>
+  </si>
+  <si>
+    <t>{R:UnitPrice}</t>
+  </si>
+  <si>
+    <t>&lt;EndTemplate Name='Products'/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Template Name='BasicVerticalWithNothingElseThanALinkedTemplate' /&gt;</t>
+  </si>
+  <si>
+    <t>&lt;EndTemplate Name='BasicVerticalWithNothingElseThanALinkedTemplate' /&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Template Name='BasicVerticalWithoutHeaderFooterAndWithLinkedTemplate' /&gt;</t>
+  </si>
+  <si>
+    <t>Template without header or footer but with a linked template</t>
+  </si>
+  <si>
+    <t>Templates used as linked templates</t>
+  </si>
+  <si>
+    <t>&lt;EndTemplate Name='BasicVerticalMultiHeaderAndFooter'/&gt;</t>
+  </si>
+  <si>
+    <t>{ME=ExcelTestTopic,Etk.Tests.Templates.ExcelDna1,GetNumberOfTests;DEC=DEC_INIT:RenderSuccessful}</t>
+  </si>
+  <si>
+    <t>Go back to Dashboard template</t>
+  </si>
+  <si>
+    <t>&lt;EndTemplate Name='GoBackToDashboard'/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Template Name='GoBackToDashboard' BindingWith='GoBackToDashBoardManager'/&gt;</t>
+  </si>
+  <si>
+    <t>[LDC=,,GoBackToDashboard:Go back to dashboard]</t>
+  </si>
+  <si>
     <t>Init Ok</t>
-  </si>
-  <si>
-    <t>{?Search...?}</t>
-  </si>
-  <si>
-    <t>Errors</t>
-  </si>
-  <si>
-    <t>{Errors}</t>
-  </si>
-  <si>
-    <t>[LDC=ExcelTestsManager,,Execute:Execute All Tests]</t>
-  </si>
-  <si>
-    <t>&lt;Link To='TestTopics' With='TestTopics' /&gt;</t>
-  </si>
-  <si>
-    <t>&lt;EndTemplate Name='TestTopics'/&gt;</t>
-  </si>
-  <si>
-    <t>[ME=ExcelTestTopic,,GetNumberOfTests;LDC=ExcelTestTopic,,Execute:Execute]</t>
-  </si>
-  <si>
-    <t>{ME=ExcelTestTopic,,GetNumberOfTests:Exception}</t>
-  </si>
-  <si>
-    <t>Definition of the Decorators</t>
-  </si>
-  <si>
-    <t>DEC_STATUS</t>
-  </si>
-  <si>
-    <t>Text</t>
-  </si>
-  <si>
-    <t>DEC_INIT</t>
-  </si>
-  <si>
-    <t>DEC_EXEC</t>
-  </si>
-  <si>
-    <t>DEC_DONE</t>
-  </si>
-  <si>
-    <t>{DEC=DEC_STATUS:Status}</t>
-  </si>
-  <si>
-    <t>{ME=ExcelTestTopic,Etk.Tests.Templates.ExcelDna1,GetNumberOfTests;DEC=DEC_INIT:InitSuccessful}</t>
-  </si>
-  <si>
-    <t>{DEC=DEC_DONE:Done}</t>
-  </si>
-  <si>
-    <t>{DEC=DEC_EXEC:Success}</t>
-  </si>
-  <si>
-    <t>&lt;Template Name='Main' BindingWith='ExcelTestsManager'/&gt;</t>
-  </si>
-  <si>
-    <t>{ME=ExcelTestTopic,,GetNumberOfTests;LDC=ExcelTestsManager,Etk.Tests.Templates.ExcelDna1,SetSearchValue:Description}</t>
-  </si>
-  <si>
-    <t>{LDC=ExcelTest,Etk.Tests.Templates.ExcelDna1,DisplayResultSheet:Description}</t>
-  </si>
-  <si>
-    <t>&lt;Template Name='TestTopics' BindingWith='IExcelTestTopic' /&gt;</t>
-  </si>
-  <si>
-    <t>Basic vertical templates (without linked templates)</t>
-  </si>
-  <si>
-    <t>Vertical templates with linked templates</t>
-  </si>
-  <si>
-    <t>Template with only a linked template</t>
-  </si>
-  <si>
-    <t>&lt;Link To='Products' With='GetAllProducts' /&gt;</t>
-  </si>
-  <si>
-    <t>&lt;Template Name='Products' BindingWith='Product' /&gt;</t>
-  </si>
-  <si>
-    <t>{R:Name}</t>
-  </si>
-  <si>
-    <t>{R:UnitPrice}</t>
-  </si>
-  <si>
-    <t>&lt;EndTemplate Name='Products'/&gt;</t>
-  </si>
-  <si>
-    <t>&lt;Template Name='BasicVerticalWithNothingElseThanALinkedTemplate' /&gt;</t>
-  </si>
-  <si>
-    <t>&lt;EndTemplate Name='BasicVerticalWithNothingElseThanALinkedTemplate' /&gt;</t>
-  </si>
-  <si>
-    <t>&lt;Template Name='BasicVerticalWithoutHeaderFooterAndWithLinkedTemplate' /&gt;</t>
-  </si>
-  <si>
-    <t>Template without header or footer but with a linked template</t>
-  </si>
-  <si>
-    <t>Templates used as linked templates</t>
-  </si>
-  <si>
-    <t>&lt;EndTemplate Name='BasicVerticalMultiHeaderAndFooter'/&gt;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -508,6 +571,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
@@ -676,7 +746,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="22">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -873,21 +943,6 @@
         <color indexed="64"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
         <color indexed="64"/>
       </right>
       <top style="medium">
@@ -937,7 +992,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="1" fontId="0" fillId="5" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -998,19 +1053,13 @@
     <xf numFmtId="0" fontId="2" fillId="19" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1019,7 +1068,7 @@
     <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1" applyProtection="1">
@@ -1056,18 +1105,6 @@
     <xf numFmtId="0" fontId="2" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1077,7 +1114,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1440,25 +1477,25 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="30"/>
-    <col min="2" max="2" width="15.85546875" style="30" customWidth="1"/>
-    <col min="3" max="3" width="88.7109375" style="30" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.85546875" style="30" customWidth="1"/>
-    <col min="5" max="5" width="9.7109375" style="30" customWidth="1"/>
-    <col min="6" max="6" width="100.7109375" style="30" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.7109375" style="30" customWidth="1"/>
-    <col min="8" max="8" width="7.7109375" style="30" customWidth="1"/>
-    <col min="9" max="9" width="6.140625" style="30" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.28515625" style="30" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10" style="30" bestFit="1" customWidth="1"/>
-    <col min="12" max="14" width="11.42578125" style="30"/>
-    <col min="15" max="15" width="2.42578125" style="30" bestFit="1" customWidth="1"/>
-    <col min="16" max="16384" width="11.42578125" style="30"/>
+    <col min="1" max="1" width="11.42578125" style="28"/>
+    <col min="2" max="2" width="15.85546875" style="28" customWidth="1"/>
+    <col min="3" max="3" width="88.7109375" style="28" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.85546875" style="28" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" style="28" customWidth="1"/>
+    <col min="6" max="6" width="100.7109375" style="28" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.7109375" style="28" customWidth="1"/>
+    <col min="8" max="8" width="7.7109375" style="28" customWidth="1"/>
+    <col min="9" max="9" width="6.140625" style="28" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.28515625" style="28" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10" style="28" bestFit="1" customWidth="1"/>
+    <col min="12" max="14" width="11.42578125" style="28"/>
+    <col min="15" max="15" width="2.42578125" style="28" bestFit="1" customWidth="1"/>
+    <col min="16" max="16384" width="11.42578125" style="28"/>
   </cols>
   <sheetData>
     <row r="2" spans="14:15" x14ac:dyDescent="0.25">
-      <c r="N2" s="32"/>
-      <c r="O2" s="32"/>
+      <c r="N2" s="30"/>
+      <c r="O2" s="30"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" autoFilter="0" pivotTables="0"/>
@@ -1472,10 +1509,10 @@
   <sheetPr>
     <tabColor theme="4" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:P21"/>
+  <dimension ref="A1:P28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1484,7 +1521,7 @@
     <col min="2" max="2" width="85.28515625" customWidth="1"/>
     <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="79.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.7109375" customWidth="1"/>
+    <col min="5" max="5" width="73" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="66.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.5703125" bestFit="1" customWidth="1"/>
@@ -1495,197 +1532,214 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="30"/>
+      <c r="A1" s="28"/>
     </row>
     <row r="3" spans="1:16" ht="21" x14ac:dyDescent="0.25">
-      <c r="A3" s="47" t="s">
+      <c r="A3" s="41" t="s">
         <v>77</v>
       </c>
-      <c r="B3" s="48"/>
-      <c r="C3" s="48"/>
-      <c r="D3" s="48"/>
-      <c r="E3" s="48"/>
-      <c r="F3" s="48"/>
-      <c r="G3" s="48"/>
-      <c r="H3" s="48"/>
-      <c r="I3" s="48"/>
-      <c r="J3" s="48"/>
-      <c r="K3" s="48"/>
-      <c r="L3" s="48"/>
-      <c r="M3" s="48"/>
-      <c r="N3" s="48"/>
-      <c r="O3" s="48"/>
-      <c r="P3" s="49"/>
+      <c r="B3" s="42"/>
+      <c r="C3" s="42"/>
+      <c r="D3" s="42"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="42"/>
+      <c r="G3" s="42"/>
+      <c r="H3" s="42"/>
+      <c r="I3" s="42"/>
+      <c r="J3" s="42"/>
+      <c r="K3" s="42"/>
+      <c r="L3" s="42"/>
+      <c r="M3" s="42"/>
+      <c r="N3" s="42"/>
+      <c r="O3" s="42"/>
+      <c r="P3" s="43"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="39" t="s">
-        <v>102</v>
-      </c>
-      <c r="C5" s="34" t="s">
-        <v>88</v>
-      </c>
-      <c r="D5" s="30"/>
-      <c r="E5" s="30"/>
-      <c r="F5" s="30"/>
-      <c r="G5" s="30"/>
-      <c r="H5" s="30"/>
-      <c r="I5" s="30"/>
-      <c r="J5" s="30"/>
-      <c r="K5" s="30"/>
+      <c r="B5" s="37" t="s">
+        <v>97</v>
+      </c>
+      <c r="C5" s="32" t="s">
+        <v>86</v>
+      </c>
+      <c r="D5" s="28"/>
+      <c r="E5" s="28"/>
+      <c r="F5" s="28"/>
+      <c r="G5" s="28"/>
     </row>
     <row r="6" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>79</v>
       </c>
-      <c r="B6" s="37" t="s">
-        <v>91</v>
-      </c>
-      <c r="C6" s="31" t="s">
+      <c r="B6" s="35" t="s">
+        <v>87</v>
+      </c>
+      <c r="C6" s="29" t="s">
         <v>80</v>
       </c>
       <c r="D6" s="23" t="s">
-        <v>87</v>
-      </c>
-      <c r="E6" s="24" t="s">
+        <v>123</v>
+      </c>
+      <c r="E6" s="27" t="s">
+        <v>80</v>
+      </c>
+      <c r="F6" s="26" t="s">
         <v>82</v>
       </c>
-      <c r="F6" s="29" t="s">
-        <v>80</v>
-      </c>
-      <c r="G6" s="28" t="s">
-        <v>83</v>
-      </c>
-      <c r="H6" s="25" t="s">
+      <c r="G6" s="24" t="s">
         <v>81</v>
       </c>
-      <c r="I6" s="26" t="s">
-        <v>89</v>
-      </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B7" s="30" t="s">
-        <v>92</v>
-      </c>
-      <c r="C7" s="30"/>
-      <c r="D7" s="30"/>
-      <c r="E7" s="30"/>
-      <c r="F7" s="30"/>
-      <c r="G7" s="30"/>
-      <c r="H7" s="30"/>
-      <c r="I7" s="30"/>
-      <c r="J7" s="1" t="s">
+      <c r="B7" s="28" t="s">
+        <v>88</v>
+      </c>
+      <c r="C7" s="28"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
+      <c r="F7" s="28"/>
+      <c r="G7" s="28"/>
+      <c r="H7" s="1" t="s">
         <v>78</v>
       </c>
+      <c r="I7" s="28"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B10" s="33" t="s">
+      <c r="B10" s="31" t="s">
+        <v>90</v>
+      </c>
+      <c r="C10" s="34" t="s">
+        <v>101</v>
+      </c>
+      <c r="D10" s="33" t="s">
+        <v>118</v>
+      </c>
+      <c r="E10" s="28" t="s">
+        <v>83</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="D12" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="E13" s="25" t="s">
+        <v>102</v>
+      </c>
+      <c r="F13" s="25" t="s">
+        <v>98</v>
+      </c>
+      <c r="G13" s="25" t="s">
+        <v>99</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="44" t="s">
+        <v>91</v>
+      </c>
+      <c r="B18" s="45"/>
+      <c r="C18" s="45"/>
+      <c r="D18" s="45"/>
+    </row>
+    <row r="19" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="36" t="s">
+        <v>92</v>
+      </c>
+      <c r="B19" s="36" t="s">
         <v>94</v>
       </c>
-      <c r="C10" s="36" t="s">
-        <v>107</v>
-      </c>
-      <c r="D10" s="35" t="s">
-        <v>103</v>
-      </c>
-      <c r="E10" s="35" t="s">
+      <c r="C19" s="36" t="s">
+        <v>96</v>
+      </c>
+      <c r="D19" s="36" t="s">
         <v>95</v>
       </c>
-      <c r="F10" s="30" t="s">
-        <v>84</v>
-      </c>
-      <c r="G10" s="1" t="s">
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A20" s="37" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="E12" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="F13" s="27" t="s">
-        <v>108</v>
-      </c>
-      <c r="G13" s="27" t="s">
-        <v>104</v>
-      </c>
-      <c r="H13" s="27" t="s">
-        <v>105</v>
-      </c>
-      <c r="I13" s="27" t="s">
-        <v>90</v>
-      </c>
-      <c r="J13" s="1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="50" t="s">
-        <v>96</v>
-      </c>
-      <c r="B18" s="51"/>
-      <c r="C18" s="51"/>
-      <c r="D18" s="51"/>
-    </row>
-    <row r="19" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="38" t="s">
-        <v>97</v>
-      </c>
-      <c r="B19" s="38" t="s">
-        <v>99</v>
-      </c>
-      <c r="C19" s="38" t="s">
-        <v>101</v>
-      </c>
-      <c r="D19" s="38" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="39" t="s">
-        <v>98</v>
-      </c>
-      <c r="B20" s="35" t="s">
-        <v>98</v>
-      </c>
-      <c r="C20" s="27" t="s">
-        <v>98</v>
-      </c>
-      <c r="D20" s="27" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="40" t="s">
-        <v>98</v>
-      </c>
-      <c r="B21" s="41" t="s">
-        <v>98</v>
-      </c>
-      <c r="C21" s="41" t="s">
-        <v>98</v>
-      </c>
-      <c r="D21" s="41" t="s">
-        <v>98</v>
+      <c r="B20" s="33" t="s">
+        <v>93</v>
+      </c>
+      <c r="C20" s="25" t="s">
+        <v>93</v>
+      </c>
+      <c r="D20" s="25" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A21" s="38" t="s">
+        <v>93</v>
+      </c>
+      <c r="B21" s="39" t="s">
+        <v>93</v>
+      </c>
+      <c r="C21" s="39" t="s">
+        <v>93</v>
+      </c>
+      <c r="D21" s="39" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" ht="21" x14ac:dyDescent="0.25">
+      <c r="A25" s="41" t="s">
+        <v>119</v>
+      </c>
+      <c r="B25" s="42"/>
+      <c r="C25" s="42"/>
+      <c r="D25" s="42"/>
+      <c r="E25" s="42"/>
+      <c r="F25" s="42"/>
+      <c r="G25" s="42"/>
+      <c r="H25" s="42"/>
+      <c r="I25" s="42"/>
+      <c r="J25" s="42"/>
+      <c r="K25" s="42"/>
+      <c r="L25" s="42"/>
+      <c r="M25" s="42"/>
+      <c r="N25" s="42"/>
+      <c r="O25" s="42"/>
+      <c r="P25" s="43"/>
+    </row>
+    <row r="27" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="35" t="s">
+        <v>122</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>120</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A3:P3"/>
     <mergeCell ref="A18:D18"/>
+    <mergeCell ref="A25:P25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1698,186 +1752,181 @@
   <sheetPr>
     <tabColor theme="4" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:S23"/>
+  <dimension ref="A2:S23"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A1" s="30"/>
-    </row>
     <row r="2" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:19" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="52" t="s">
+      <c r="A3" s="46" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="53"/>
-      <c r="C3" s="53"/>
-      <c r="D3" s="53"/>
-      <c r="E3" s="53"/>
-      <c r="F3" s="53"/>
-      <c r="G3" s="53"/>
-      <c r="H3" s="53"/>
-      <c r="I3" s="53"/>
-      <c r="J3" s="53"/>
-      <c r="K3" s="53"/>
-      <c r="L3" s="53"/>
-      <c r="M3" s="53"/>
-      <c r="N3" s="53"/>
-      <c r="O3" s="53"/>
-      <c r="P3" s="54"/>
+      <c r="B3" s="47"/>
+      <c r="C3" s="47"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="47"/>
+      <c r="F3" s="47"/>
+      <c r="G3" s="47"/>
+      <c r="H3" s="47"/>
+      <c r="I3" s="47"/>
+      <c r="J3" s="47"/>
+      <c r="K3" s="47"/>
+      <c r="L3" s="47"/>
+      <c r="M3" s="47"/>
+      <c r="N3" s="47"/>
+      <c r="O3" s="47"/>
+      <c r="P3" s="48"/>
     </row>
     <row r="5" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I5" s="55" t="s">
+      <c r="I5" s="49" t="s">
         <v>20</v>
       </c>
-      <c r="J5" s="56"/>
-      <c r="K5" s="56"/>
-      <c r="L5" s="56"/>
-      <c r="M5" s="56"/>
-      <c r="N5" s="56"/>
-      <c r="O5" s="56"/>
-      <c r="P5" s="56"/>
-      <c r="Q5" s="56"/>
-      <c r="R5" s="56"/>
-      <c r="S5" s="57"/>
+      <c r="J5" s="50"/>
+      <c r="K5" s="50"/>
+      <c r="L5" s="50"/>
+      <c r="M5" s="50"/>
+      <c r="N5" s="50"/>
+      <c r="O5" s="50"/>
+      <c r="P5" s="50"/>
+      <c r="Q5" s="50"/>
+      <c r="R5" s="50"/>
+      <c r="S5" s="51"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="I6" s="58" t="s">
+      <c r="I6" s="52" t="s">
         <v>27</v>
       </c>
-      <c r="J6" s="59"/>
-      <c r="K6" s="59"/>
-      <c r="L6" s="59"/>
-      <c r="M6" s="59"/>
-      <c r="N6" s="59"/>
-      <c r="O6" s="59"/>
-      <c r="P6" s="59"/>
-      <c r="Q6" s="59"/>
-      <c r="R6" s="59"/>
-      <c r="S6" s="60"/>
+      <c r="J6" s="53"/>
+      <c r="K6" s="53"/>
+      <c r="L6" s="53"/>
+      <c r="M6" s="53"/>
+      <c r="N6" s="53"/>
+      <c r="O6" s="53"/>
+      <c r="P6" s="53"/>
+      <c r="Q6" s="53"/>
+      <c r="R6" s="53"/>
+      <c r="S6" s="54"/>
     </row>
     <row r="7" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I7" s="61" t="s">
+      <c r="I7" s="55" t="s">
         <v>26</v>
       </c>
-      <c r="J7" s="62"/>
-      <c r="K7" s="62"/>
-      <c r="L7" s="62"/>
-      <c r="M7" s="62"/>
-      <c r="N7" s="62"/>
-      <c r="O7" s="62"/>
-      <c r="P7" s="62"/>
-      <c r="Q7" s="62"/>
-      <c r="R7" s="62"/>
-      <c r="S7" s="63"/>
+      <c r="J7" s="56"/>
+      <c r="K7" s="56"/>
+      <c r="L7" s="56"/>
+      <c r="M7" s="56"/>
+      <c r="N7" s="56"/>
+      <c r="O7" s="56"/>
+      <c r="P7" s="56"/>
+      <c r="Q7" s="56"/>
+      <c r="R7" s="56"/>
+      <c r="S7" s="57"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="I10" s="55" t="s">
+      <c r="I10" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="J10" s="56"/>
-      <c r="K10" s="56"/>
-      <c r="L10" s="56"/>
-      <c r="M10" s="56"/>
-      <c r="N10" s="56"/>
-      <c r="O10" s="56"/>
-      <c r="P10" s="56"/>
-      <c r="Q10" s="56"/>
-      <c r="R10" s="56"/>
-      <c r="S10" s="57"/>
+      <c r="J10" s="50"/>
+      <c r="K10" s="50"/>
+      <c r="L10" s="50"/>
+      <c r="M10" s="50"/>
+      <c r="N10" s="50"/>
+      <c r="O10" s="50"/>
+      <c r="P10" s="50"/>
+      <c r="Q10" s="50"/>
+      <c r="R10" s="50"/>
+      <c r="S10" s="51"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="I11" s="58" t="s">
+      <c r="I11" s="52" t="s">
         <v>27</v>
       </c>
-      <c r="J11" s="59"/>
-      <c r="K11" s="59"/>
-      <c r="L11" s="59"/>
-      <c r="M11" s="59"/>
-      <c r="N11" s="59"/>
-      <c r="O11" s="59"/>
-      <c r="P11" s="59"/>
-      <c r="Q11" s="59"/>
-      <c r="R11" s="59"/>
-      <c r="S11" s="60"/>
+      <c r="J11" s="53"/>
+      <c r="K11" s="53"/>
+      <c r="L11" s="53"/>
+      <c r="M11" s="53"/>
+      <c r="N11" s="53"/>
+      <c r="O11" s="53"/>
+      <c r="P11" s="53"/>
+      <c r="Q11" s="53"/>
+      <c r="R11" s="53"/>
+      <c r="S11" s="54"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="I12" s="61" t="s">
+      <c r="I12" s="55" t="s">
         <v>26</v>
       </c>
-      <c r="J12" s="62"/>
-      <c r="K12" s="62"/>
-      <c r="L12" s="62"/>
-      <c r="M12" s="62"/>
-      <c r="N12" s="62"/>
-      <c r="O12" s="62"/>
-      <c r="P12" s="62"/>
-      <c r="Q12" s="62"/>
-      <c r="R12" s="62"/>
-      <c r="S12" s="63"/>
+      <c r="J12" s="56"/>
+      <c r="K12" s="56"/>
+      <c r="L12" s="56"/>
+      <c r="M12" s="56"/>
+      <c r="N12" s="56"/>
+      <c r="O12" s="56"/>
+      <c r="P12" s="56"/>
+      <c r="Q12" s="56"/>
+      <c r="R12" s="56"/>
+      <c r="S12" s="57"/>
     </row>
     <row r="15" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="I15" s="55" t="s">
+      <c r="I15" s="49" t="s">
         <v>21</v>
       </c>
-      <c r="J15" s="56"/>
-      <c r="K15" s="56"/>
-      <c r="L15" s="56"/>
-      <c r="M15" s="56"/>
-      <c r="N15" s="56"/>
-      <c r="O15" s="56"/>
-      <c r="P15" s="56"/>
-      <c r="Q15" s="56"/>
-      <c r="R15" s="56"/>
-      <c r="S15" s="57"/>
+      <c r="J15" s="50"/>
+      <c r="K15" s="50"/>
+      <c r="L15" s="50"/>
+      <c r="M15" s="50"/>
+      <c r="N15" s="50"/>
+      <c r="O15" s="50"/>
+      <c r="P15" s="50"/>
+      <c r="Q15" s="50"/>
+      <c r="R15" s="50"/>
+      <c r="S15" s="51"/>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="I16" s="58"/>
-      <c r="J16" s="59"/>
-      <c r="K16" s="59"/>
-      <c r="L16" s="59"/>
-      <c r="M16" s="59"/>
-      <c r="N16" s="59"/>
-      <c r="O16" s="59"/>
-      <c r="P16" s="59"/>
-      <c r="Q16" s="59"/>
-      <c r="R16" s="59"/>
-      <c r="S16" s="60"/>
+      <c r="I16" s="52"/>
+      <c r="J16" s="53"/>
+      <c r="K16" s="53"/>
+      <c r="L16" s="53"/>
+      <c r="M16" s="53"/>
+      <c r="N16" s="53"/>
+      <c r="O16" s="53"/>
+      <c r="P16" s="53"/>
+      <c r="Q16" s="53"/>
+      <c r="R16" s="53"/>
+      <c r="S16" s="54"/>
     </row>
     <row r="17" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>5</v>
       </c>
-      <c r="I17" s="61"/>
-      <c r="J17" s="62"/>
-      <c r="K17" s="62"/>
-      <c r="L17" s="62"/>
-      <c r="M17" s="62"/>
-      <c r="N17" s="62"/>
-      <c r="O17" s="62"/>
-      <c r="P17" s="62"/>
-      <c r="Q17" s="62"/>
-      <c r="R17" s="62"/>
-      <c r="S17" s="63"/>
+      <c r="I17" s="55"/>
+      <c r="J17" s="56"/>
+      <c r="K17" s="56"/>
+      <c r="L17" s="56"/>
+      <c r="M17" s="56"/>
+      <c r="N17" s="56"/>
+      <c r="O17" s="56"/>
+      <c r="P17" s="56"/>
+      <c r="Q17" s="56"/>
+      <c r="R17" s="56"/>
+      <c r="S17" s="57"/>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C18" s="1" t="s">
@@ -1891,48 +1940,48 @@
       <c r="C21" t="s">
         <v>5</v>
       </c>
-      <c r="I21" s="55" t="s">
+      <c r="I21" s="49" t="s">
         <v>24</v>
       </c>
-      <c r="J21" s="56"/>
-      <c r="K21" s="56"/>
-      <c r="L21" s="56"/>
-      <c r="M21" s="56"/>
-      <c r="N21" s="56"/>
-      <c r="O21" s="56"/>
-      <c r="P21" s="56"/>
-      <c r="Q21" s="56"/>
-      <c r="R21" s="56"/>
-      <c r="S21" s="57"/>
+      <c r="J21" s="50"/>
+      <c r="K21" s="50"/>
+      <c r="L21" s="50"/>
+      <c r="M21" s="50"/>
+      <c r="N21" s="50"/>
+      <c r="O21" s="50"/>
+      <c r="P21" s="50"/>
+      <c r="Q21" s="50"/>
+      <c r="R21" s="50"/>
+      <c r="S21" s="51"/>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="I22" s="58"/>
-      <c r="J22" s="59"/>
-      <c r="K22" s="59"/>
-      <c r="L22" s="59"/>
-      <c r="M22" s="59"/>
-      <c r="N22" s="59"/>
-      <c r="O22" s="59"/>
-      <c r="P22" s="59"/>
-      <c r="Q22" s="59"/>
-      <c r="R22" s="59"/>
-      <c r="S22" s="60"/>
+      <c r="I22" s="52"/>
+      <c r="J22" s="53"/>
+      <c r="K22" s="53"/>
+      <c r="L22" s="53"/>
+      <c r="M22" s="53"/>
+      <c r="N22" s="53"/>
+      <c r="O22" s="53"/>
+      <c r="P22" s="53"/>
+      <c r="Q22" s="53"/>
+      <c r="R22" s="53"/>
+      <c r="S22" s="54"/>
     </row>
     <row r="23" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C23" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="I23" s="61"/>
-      <c r="J23" s="62"/>
-      <c r="K23" s="62"/>
-      <c r="L23" s="62"/>
-      <c r="M23" s="62"/>
-      <c r="N23" s="62"/>
-      <c r="O23" s="62"/>
-      <c r="P23" s="62"/>
-      <c r="Q23" s="62"/>
-      <c r="R23" s="62"/>
-      <c r="S23" s="63"/>
+      <c r="I23" s="55"/>
+      <c r="J23" s="56"/>
+      <c r="K23" s="56"/>
+      <c r="L23" s="56"/>
+      <c r="M23" s="56"/>
+      <c r="N23" s="56"/>
+      <c r="O23" s="56"/>
+      <c r="P23" s="56"/>
+      <c r="Q23" s="56"/>
+      <c r="R23" s="56"/>
+      <c r="S23" s="57"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -1956,11 +2005,9 @@
   <sheetPr>
     <tabColor theme="4" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:S59"/>
+  <dimension ref="A3:Q73"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1973,48 +2020,45 @@
     <col min="14" max="14" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="30"/>
-    </row>
     <row r="3" spans="1:16" ht="21" x14ac:dyDescent="0.25">
-      <c r="A3" s="47" t="s">
-        <v>110</v>
-      </c>
-      <c r="B3" s="48"/>
-      <c r="C3" s="48"/>
-      <c r="D3" s="48"/>
-      <c r="E3" s="48"/>
-      <c r="F3" s="48"/>
-      <c r="G3" s="48"/>
-      <c r="H3" s="48"/>
-      <c r="I3" s="48"/>
-      <c r="J3" s="48"/>
-      <c r="K3" s="48"/>
-      <c r="L3" s="48"/>
-      <c r="M3" s="48"/>
-      <c r="N3" s="48"/>
-      <c r="O3" s="48"/>
-      <c r="P3" s="49"/>
+      <c r="A3" s="41" t="s">
+        <v>104</v>
+      </c>
+      <c r="B3" s="42"/>
+      <c r="C3" s="42"/>
+      <c r="D3" s="42"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="42"/>
+      <c r="G3" s="42"/>
+      <c r="H3" s="42"/>
+      <c r="I3" s="42"/>
+      <c r="J3" s="42"/>
+      <c r="K3" s="42"/>
+      <c r="L3" s="42"/>
+      <c r="M3" s="42"/>
+      <c r="N3" s="42"/>
+      <c r="O3" s="42"/>
+      <c r="P3" s="43"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="67" t="s">
+      <c r="A4" s="61" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="68"/>
-      <c r="C4" s="68"/>
-      <c r="D4" s="68"/>
-      <c r="E4" s="68"/>
-      <c r="F4" s="68"/>
-      <c r="G4" s="68"/>
-      <c r="H4" s="68"/>
-      <c r="I4" s="68"/>
-      <c r="J4" s="68"/>
-      <c r="K4" s="68"/>
-      <c r="L4" s="68"/>
-      <c r="M4" s="68"/>
-      <c r="N4" s="68"/>
-      <c r="O4" s="68"/>
-      <c r="P4" s="69"/>
+      <c r="B4" s="62"/>
+      <c r="C4" s="62"/>
+      <c r="D4" s="62"/>
+      <c r="E4" s="62"/>
+      <c r="F4" s="62"/>
+      <c r="G4" s="62"/>
+      <c r="H4" s="62"/>
+      <c r="I4" s="62"/>
+      <c r="J4" s="62"/>
+      <c r="K4" s="62"/>
+      <c r="L4" s="62"/>
+      <c r="M4" s="62"/>
+      <c r="N4" s="62"/>
+      <c r="O4" s="62"/>
+      <c r="P4" s="63"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
@@ -2039,24 +2083,24 @@
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" s="67" t="s">
+      <c r="A8" s="61" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="68"/>
-      <c r="C8" s="68"/>
-      <c r="D8" s="68"/>
-      <c r="E8" s="68"/>
-      <c r="F8" s="68"/>
-      <c r="G8" s="68"/>
-      <c r="H8" s="68"/>
-      <c r="I8" s="68"/>
-      <c r="J8" s="68"/>
-      <c r="K8" s="68"/>
-      <c r="L8" s="68"/>
-      <c r="M8" s="68"/>
-      <c r="N8" s="68"/>
-      <c r="O8" s="68"/>
-      <c r="P8" s="69"/>
+      <c r="B8" s="62"/>
+      <c r="C8" s="62"/>
+      <c r="D8" s="62"/>
+      <c r="E8" s="62"/>
+      <c r="F8" s="62"/>
+      <c r="G8" s="62"/>
+      <c r="H8" s="62"/>
+      <c r="I8" s="62"/>
+      <c r="J8" s="62"/>
+      <c r="K8" s="62"/>
+      <c r="L8" s="62"/>
+      <c r="M8" s="62"/>
+      <c r="N8" s="62"/>
+      <c r="O8" s="62"/>
+      <c r="P8" s="63"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
@@ -2099,35 +2143,35 @@
       <c r="A12" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B12" s="70" t="s">
+      <c r="B12" s="64" t="s">
         <v>35</v>
       </c>
-      <c r="C12" s="71"/>
-      <c r="D12" s="71"/>
-      <c r="E12" s="72"/>
+      <c r="C12" s="65"/>
+      <c r="D12" s="65"/>
+      <c r="E12" s="66"/>
       <c r="F12" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" s="67" t="s">
+      <c r="A15" s="61" t="s">
         <v>6</v>
       </c>
-      <c r="B15" s="68"/>
-      <c r="C15" s="68"/>
-      <c r="D15" s="68"/>
-      <c r="E15" s="68"/>
-      <c r="F15" s="68"/>
-      <c r="G15" s="68"/>
-      <c r="H15" s="68"/>
-      <c r="I15" s="68"/>
-      <c r="J15" s="68"/>
-      <c r="K15" s="68"/>
-      <c r="L15" s="68"/>
-      <c r="M15" s="68"/>
-      <c r="N15" s="68"/>
-      <c r="O15" s="68"/>
-      <c r="P15" s="69"/>
+      <c r="B15" s="62"/>
+      <c r="C15" s="62"/>
+      <c r="D15" s="62"/>
+      <c r="E15" s="62"/>
+      <c r="F15" s="62"/>
+      <c r="G15" s="62"/>
+      <c r="H15" s="62"/>
+      <c r="I15" s="62"/>
+      <c r="J15" s="62"/>
+      <c r="K15" s="62"/>
+      <c r="L15" s="62"/>
+      <c r="M15" s="62"/>
+      <c r="N15" s="62"/>
+      <c r="O15" s="62"/>
+      <c r="P15" s="63"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
@@ -2138,12 +2182,12 @@
       <c r="A17" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B17" s="70" t="s">
+      <c r="B17" s="64" t="s">
         <v>35</v>
       </c>
-      <c r="C17" s="71"/>
-      <c r="D17" s="71"/>
-      <c r="E17" s="72"/>
+      <c r="C17" s="65"/>
+      <c r="D17" s="65"/>
+      <c r="E17" s="66"/>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
@@ -2181,70 +2225,70 @@
       <c r="A20" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B20" s="70" t="s">
+      <c r="B20" s="64" t="s">
         <v>36</v>
       </c>
-      <c r="C20" s="71"/>
-      <c r="D20" s="71"/>
-      <c r="E20" s="72"/>
+      <c r="C20" s="65"/>
+      <c r="D20" s="65"/>
+      <c r="E20" s="66"/>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B21" s="70" t="s">
+      <c r="B21" s="64" t="s">
         <v>35</v>
       </c>
-      <c r="C21" s="71"/>
-      <c r="D21" s="71"/>
-      <c r="E21" s="72"/>
+      <c r="C21" s="65"/>
+      <c r="D21" s="65"/>
+      <c r="E21" s="66"/>
       <c r="F21" s="1" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
     </row>
     <row r="26" spans="1:16" ht="21" x14ac:dyDescent="0.25">
-      <c r="A26" s="47" t="s">
-        <v>111</v>
-      </c>
-      <c r="B26" s="48"/>
-      <c r="C26" s="48"/>
-      <c r="D26" s="48"/>
-      <c r="E26" s="48"/>
-      <c r="F26" s="48"/>
-      <c r="G26" s="48"/>
-      <c r="H26" s="48"/>
-      <c r="I26" s="48"/>
-      <c r="J26" s="48"/>
-      <c r="K26" s="48"/>
-      <c r="L26" s="48"/>
-      <c r="M26" s="48"/>
-      <c r="N26" s="48"/>
-      <c r="O26" s="48"/>
-      <c r="P26" s="49"/>
+      <c r="A26" s="41" t="s">
+        <v>105</v>
+      </c>
+      <c r="B26" s="42"/>
+      <c r="C26" s="42"/>
+      <c r="D26" s="42"/>
+      <c r="E26" s="42"/>
+      <c r="F26" s="42"/>
+      <c r="G26" s="42"/>
+      <c r="H26" s="42"/>
+      <c r="I26" s="42"/>
+      <c r="J26" s="42"/>
+      <c r="K26" s="42"/>
+      <c r="L26" s="42"/>
+      <c r="M26" s="42"/>
+      <c r="N26" s="42"/>
+      <c r="O26" s="42"/>
+      <c r="P26" s="43"/>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A27" s="67" t="s">
-        <v>112</v>
-      </c>
-      <c r="B27" s="68"/>
-      <c r="C27" s="68"/>
-      <c r="D27" s="68"/>
-      <c r="E27" s="68"/>
-      <c r="F27" s="68"/>
-      <c r="G27" s="68"/>
-      <c r="H27" s="68"/>
-      <c r="I27" s="68"/>
-      <c r="J27" s="68"/>
-      <c r="K27" s="68"/>
-      <c r="L27" s="68"/>
-      <c r="M27" s="68"/>
-      <c r="N27" s="68"/>
-      <c r="O27" s="68"/>
-      <c r="P27" s="69"/>
+      <c r="A27" s="61" t="s">
+        <v>106</v>
+      </c>
+      <c r="B27" s="62"/>
+      <c r="C27" s="62"/>
+      <c r="D27" s="62"/>
+      <c r="E27" s="62"/>
+      <c r="F27" s="62"/>
+      <c r="G27" s="62"/>
+      <c r="H27" s="62"/>
+      <c r="I27" s="62"/>
+      <c r="J27" s="62"/>
+      <c r="K27" s="62"/>
+      <c r="L27" s="62"/>
+      <c r="M27" s="62"/>
+      <c r="N27" s="62"/>
+      <c r="O27" s="62"/>
+      <c r="P27" s="63"/>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="F29" s="15"/>
       <c r="G29" s="15"/>
@@ -2259,10 +2303,10 @@
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C30" s="1" t="s">
         <v>113</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>119</v>
       </c>
       <c r="F30" s="15"/>
       <c r="G30" s="15"/>
@@ -2287,39 +2331,39 @@
       <c r="N31" s="15"/>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A32" s="67" t="s">
-        <v>121</v>
-      </c>
-      <c r="B32" s="68"/>
-      <c r="C32" s="68"/>
-      <c r="D32" s="68"/>
-      <c r="E32" s="68"/>
-      <c r="F32" s="68"/>
-      <c r="G32" s="68"/>
-      <c r="H32" s="68"/>
-      <c r="I32" s="68"/>
-      <c r="J32" s="68"/>
-      <c r="K32" s="68"/>
-      <c r="L32" s="68"/>
-      <c r="M32" s="68"/>
-      <c r="N32" s="68"/>
-      <c r="O32" s="68"/>
-      <c r="P32" s="69"/>
-    </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A32" s="61" t="s">
+        <v>115</v>
+      </c>
+      <c r="B32" s="62"/>
+      <c r="C32" s="62"/>
+      <c r="D32" s="62"/>
+      <c r="E32" s="62"/>
+      <c r="F32" s="62"/>
+      <c r="G32" s="62"/>
+      <c r="H32" s="62"/>
+      <c r="I32" s="62"/>
+      <c r="J32" s="62"/>
+      <c r="K32" s="62"/>
+      <c r="L32" s="62"/>
+      <c r="M32" s="62"/>
+      <c r="N32" s="62"/>
+      <c r="O32" s="62"/>
+      <c r="P32" s="63"/>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="B33" s="43" t="s">
+        <v>114</v>
+      </c>
+      <c r="B33" s="64" t="s">
         <v>37</v>
       </c>
-      <c r="C33" s="44"/>
-      <c r="D33" s="44"/>
-      <c r="E33" s="45"/>
+      <c r="C33" s="65"/>
+      <c r="D33" s="65"/>
+      <c r="E33" s="66"/>
       <c r="F33" s="15"/>
       <c r="G33" s="15"/>
     </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="3" t="s">
         <v>31</v>
@@ -2343,7 +2387,7 @@
       <c r="M34" s="15"/>
       <c r="N34" s="15"/>
     </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B35" s="2" t="s">
         <v>28</v>
       </c>
@@ -2366,14 +2410,14 @@
       <c r="M35" s="15"/>
       <c r="N35" s="15"/>
     </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B36" s="42" t="s">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B36" s="40" t="s">
         <v>76</v>
       </c>
-      <c r="C36" s="42"/>
-      <c r="D36" s="42"/>
-      <c r="E36" s="42"/>
-      <c r="F36" s="42"/>
+      <c r="C36" s="40"/>
+      <c r="D36" s="40"/>
+      <c r="E36" s="40"/>
+      <c r="F36" s="40"/>
       <c r="H36" s="4"/>
       <c r="I36" s="15"/>
       <c r="J36" s="15"/>
@@ -2382,7 +2426,7 @@
       <c r="M36" s="15"/>
       <c r="N36" s="15"/>
     </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B37" s="4" t="s">
         <v>66</v>
       </c>
@@ -2399,13 +2443,13 @@
       <c r="M37" s="15"/>
       <c r="N37" s="15"/>
     </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="E38" s="15"/>
       <c r="F38" s="15"/>
       <c r="G38" s="15"/>
     </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="F39" s="15"/>
       <c r="G39" s="15"/>
@@ -2417,29 +2461,29 @@
       <c r="M39" s="15"/>
       <c r="N39" s="15"/>
     </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A40" s="67" t="s">
-        <v>122</v>
-      </c>
-      <c r="B40" s="68"/>
-      <c r="C40" s="68"/>
-      <c r="D40" s="68"/>
-      <c r="E40" s="68"/>
-      <c r="F40" s="68"/>
-      <c r="G40" s="68"/>
-      <c r="H40" s="68"/>
-      <c r="I40" s="68"/>
-      <c r="J40" s="68"/>
-      <c r="K40" s="68"/>
-      <c r="L40" s="68"/>
-      <c r="M40" s="68"/>
-      <c r="N40" s="68"/>
-      <c r="O40" s="68"/>
-      <c r="P40" s="69"/>
-    </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A40" s="61" t="s">
+        <v>116</v>
+      </c>
+      <c r="B40" s="62"/>
+      <c r="C40" s="62"/>
+      <c r="D40" s="62"/>
+      <c r="E40" s="62"/>
+      <c r="F40" s="62"/>
+      <c r="G40" s="62"/>
+      <c r="H40" s="62"/>
+      <c r="I40" s="62"/>
+      <c r="J40" s="62"/>
+      <c r="K40" s="62"/>
+      <c r="L40" s="62"/>
+      <c r="M40" s="62"/>
+      <c r="N40" s="62"/>
+      <c r="O40" s="62"/>
+      <c r="P40" s="63"/>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="B41" s="4"/>
       <c r="C41" s="4"/>
@@ -2454,19 +2498,19 @@
       <c r="M41" s="15"/>
       <c r="N41" s="15"/>
     </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A42" s="4"/>
       <c r="B42" s="11" t="s">
         <v>54</v>
       </c>
       <c r="C42" s="11" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="D42" s="12" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="H42" s="15"/>
       <c r="I42" s="15"/>
@@ -2476,12 +2520,12 @@
       <c r="M42" s="15"/>
       <c r="N42" s="15"/>
     </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="F43" s="15"/>
       <c r="G43" s="15"/>
     </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
       <c r="I44" s="15"/>
       <c r="J44" s="15"/>
       <c r="K44" s="15"/>
@@ -2492,7 +2536,7 @@
       <c r="P44" s="15"/>
       <c r="Q44" s="15"/>
     </row>
-    <row r="45" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>67</v>
       </c>
@@ -2511,7 +2555,7 @@
       <c r="N45" s="15"/>
       <c r="O45" s="15"/>
     </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B46" s="21" t="s">
         <v>39</v>
       </c>
@@ -2528,7 +2572,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B47" s="17"/>
       <c r="C47" s="18" t="s">
         <v>72</v>
@@ -2542,18 +2586,8 @@
       <c r="F47" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="L47" s="64" t="s">
-        <v>40</v>
-      </c>
-      <c r="M47" s="65"/>
-      <c r="N47" s="65"/>
-      <c r="O47" s="65"/>
-      <c r="P47" s="65"/>
-      <c r="Q47" s="65"/>
-      <c r="R47" s="65"/>
-      <c r="S47" s="66"/>
-    </row>
-    <row r="48" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B48" s="8" t="s">
         <v>33</v>
       </c>
@@ -2567,49 +2601,19 @@
         <v>68</v>
       </c>
       <c r="K48" s="4"/>
-      <c r="L48" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="M48" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="N48" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="O48" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="P48" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q48" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="R48" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="S48" s="7" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B49" s="15"/>
       <c r="C49" s="15"/>
       <c r="D49" s="16"/>
       <c r="E49" s="15"/>
       <c r="F49" s="16"/>
       <c r="K49" s="4"/>
-      <c r="L49" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="N49" s="15"/>
-      <c r="Q49" s="16"/>
-      <c r="R49" s="16"/>
-    </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H50" s="4"/>
     </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
         <v>70</v>
       </c>
@@ -2618,13 +2622,10 @@
       <c r="D51" s="4"/>
       <c r="E51" s="4"/>
       <c r="F51" s="4"/>
-      <c r="H51" s="4" t="s">
-        <v>63</v>
-      </c>
       <c r="I51" s="4"/>
       <c r="J51" s="4"/>
     </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="4"/>
       <c r="B52" s="9" t="s">
         <v>54</v>
@@ -2639,14 +2640,14 @@
         <v>57</v>
       </c>
     </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G53" s="4"/>
       <c r="H53" s="4"/>
     </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G54" s="4"/>
     </row>
-    <row r="55" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
         <v>58</v>
       </c>
@@ -2656,7 +2657,7 @@
       <c r="F55" s="4"/>
       <c r="G55" s="4"/>
     </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="4"/>
       <c r="B56" s="11" t="s">
         <v>65</v>
@@ -2677,7 +2678,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="58" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
         <v>74</v>
       </c>
@@ -2687,7 +2688,7 @@
       <c r="F58" s="4"/>
       <c r="G58" s="4"/>
     </row>
-    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="4"/>
       <c r="B59" s="11" t="s">
         <v>65</v>
@@ -2702,9 +2703,60 @@
         <v>75</v>
       </c>
     </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A69" s="58" t="s">
+        <v>40</v>
+      </c>
+      <c r="B69" s="59"/>
+      <c r="C69" s="59"/>
+      <c r="D69" s="59"/>
+      <c r="E69" s="59"/>
+      <c r="F69" s="59"/>
+      <c r="G69" s="59"/>
+      <c r="H69" s="60"/>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A70" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B70" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C70" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="D70" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="E70" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="F70" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="G70" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="H70" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A71" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="C71" s="15"/>
+      <c r="F71" s="16"/>
+      <c r="G71" s="16"/>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A73" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="13">
-    <mergeCell ref="L47:S47"/>
+  <mergeCells count="14">
+    <mergeCell ref="A69:H69"/>
     <mergeCell ref="A3:P3"/>
     <mergeCell ref="A4:P4"/>
     <mergeCell ref="A8:P8"/>
@@ -2717,437 +2769,9 @@
     <mergeCell ref="A26:P26"/>
     <mergeCell ref="A32:P32"/>
     <mergeCell ref="A40:P40"/>
+    <mergeCell ref="B33:E33"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:E9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11.42578125" style="46"/>
-    <col min="2" max="2" width="2" style="46" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" style="46" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.42578125" style="46" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="35.85546875" style="46" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="11.42578125" style="46"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2"/>
-      <c r="B2"/>
-      <c r="C2"/>
-      <c r="D2"/>
-      <c r="E2"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3"/>
-      <c r="B3"/>
-      <c r="C3"/>
-      <c r="D3"/>
-      <c r="E3"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4"/>
-      <c r="B4"/>
-      <c r="C4"/>
-      <c r="D4"/>
-      <c r="E4"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5"/>
-      <c r="B5"/>
-      <c r="C5"/>
-      <c r="D5"/>
-      <c r="E5"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6"/>
-      <c r="B6"/>
-      <c r="C6"/>
-      <c r="D6"/>
-      <c r="E6"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7"/>
-      <c r="B7"/>
-      <c r="C7"/>
-      <c r="D7"/>
-      <c r="E7"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8"/>
-      <c r="B8"/>
-      <c r="C8"/>
-      <c r="D8"/>
-      <c r="E8"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9"/>
-      <c r="B9"/>
-      <c r="C9"/>
-      <c r="D9"/>
-      <c r="E9"/>
-    </row>
-  </sheetData>
-  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" autoFilter="0" pivotTables="0"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:E10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11.42578125" style="46"/>
-    <col min="2" max="2" width="2.85546875" style="46" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" style="46" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.42578125" style="46" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="35.85546875" style="46" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="11.42578125" style="46"/>
-  </cols>
-  <sheetData>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3"/>
-      <c r="C3"/>
-      <c r="D3"/>
-      <c r="E3"/>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B4"/>
-      <c r="C4"/>
-      <c r="D4"/>
-      <c r="E4"/>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5"/>
-      <c r="C5"/>
-      <c r="D5"/>
-      <c r="E5"/>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6"/>
-      <c r="C6"/>
-      <c r="D6"/>
-      <c r="E6"/>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7"/>
-      <c r="C7"/>
-      <c r="D7"/>
-      <c r="E7"/>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B8"/>
-      <c r="C8"/>
-      <c r="D8"/>
-      <c r="E8"/>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B9"/>
-      <c r="C9"/>
-      <c r="D9"/>
-      <c r="E9"/>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B10"/>
-      <c r="C10"/>
-      <c r="D10"/>
-      <c r="E10"/>
-    </row>
-  </sheetData>
-  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" autoFilter="0" pivotTables="0"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:E10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11.42578125" style="46"/>
-    <col min="2" max="2" width="2.85546875" style="46" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" style="46" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.42578125" style="46" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="35.85546875" style="46" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="11.42578125" style="46"/>
-  </cols>
-  <sheetData>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3"/>
-      <c r="C3"/>
-      <c r="D3"/>
-      <c r="E3"/>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B4"/>
-      <c r="C4"/>
-      <c r="D4"/>
-      <c r="E4"/>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5"/>
-      <c r="C5"/>
-      <c r="D5"/>
-      <c r="E5"/>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6"/>
-      <c r="C6"/>
-      <c r="D6"/>
-      <c r="E6"/>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7"/>
-      <c r="C7"/>
-      <c r="D7"/>
-      <c r="E7"/>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B8"/>
-      <c r="C8"/>
-      <c r="D8"/>
-      <c r="E8"/>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B9"/>
-      <c r="C9"/>
-      <c r="D9"/>
-      <c r="E9"/>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B10"/>
-      <c r="C10"/>
-      <c r="D10"/>
-      <c r="E10"/>
-    </row>
-  </sheetData>
-  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" autoFilter="0" pivotTables="0"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11.42578125" style="46"/>
-    <col min="2" max="2" width="2" style="46" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" style="46" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.42578125" style="46" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="35.85546875" style="46" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="11.42578125" style="46"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B2"/>
-      <c r="C2"/>
-      <c r="D2"/>
-      <c r="E2"/>
-    </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3"/>
-      <c r="C3"/>
-      <c r="D3"/>
-      <c r="E3"/>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B4"/>
-      <c r="C4"/>
-      <c r="D4"/>
-      <c r="E4"/>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5"/>
-      <c r="C5"/>
-      <c r="D5"/>
-      <c r="E5"/>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6"/>
-      <c r="C6"/>
-      <c r="D6"/>
-      <c r="E6"/>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7"/>
-      <c r="C7"/>
-      <c r="D7"/>
-      <c r="E7"/>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B8"/>
-      <c r="C8"/>
-      <c r="D8"/>
-      <c r="E8"/>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B9"/>
-      <c r="C9"/>
-      <c r="D9"/>
-      <c r="E9"/>
-    </row>
-  </sheetData>
-  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" autoFilter="0" pivotTables="0"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:F16"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11.42578125" style="46"/>
-    <col min="2" max="2" width="3" style="46" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.28515625" style="46" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.5703125" style="46" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="11.42578125" style="46"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2"/>
-      <c r="B2"/>
-      <c r="C2"/>
-      <c r="D2"/>
-      <c r="E2"/>
-      <c r="F2"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3"/>
-      <c r="B3"/>
-      <c r="C3"/>
-      <c r="D3"/>
-      <c r="E3"/>
-      <c r="F3"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4"/>
-      <c r="B4"/>
-      <c r="C4"/>
-      <c r="D4"/>
-      <c r="E4"/>
-      <c r="F4"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5"/>
-      <c r="B5"/>
-      <c r="C5"/>
-      <c r="D5"/>
-      <c r="E5"/>
-      <c r="F5"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6"/>
-      <c r="B6"/>
-      <c r="C6"/>
-      <c r="D6"/>
-      <c r="E6"/>
-      <c r="F6"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7"/>
-      <c r="B7"/>
-      <c r="C7"/>
-      <c r="D7"/>
-      <c r="E7"/>
-      <c r="F7"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8"/>
-      <c r="B8"/>
-      <c r="C8"/>
-      <c r="D8"/>
-      <c r="E8"/>
-      <c r="F8"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9"/>
-      <c r="B9"/>
-      <c r="C9"/>
-      <c r="D9"/>
-      <c r="E9"/>
-      <c r="F9"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10"/>
-      <c r="B10"/>
-      <c r="C10"/>
-      <c r="D10"/>
-      <c r="E10"/>
-      <c r="F10"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11"/>
-      <c r="B11"/>
-      <c r="C11"/>
-      <c r="D11"/>
-      <c r="E11"/>
-      <c r="F11"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12"/>
-      <c r="B12"/>
-      <c r="C12"/>
-      <c r="D12"/>
-      <c r="E12"/>
-      <c r="F12"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13"/>
-      <c r="B13"/>
-      <c r="C13"/>
-      <c r="D13"/>
-      <c r="E13"/>
-      <c r="F13"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14"/>
-      <c r="B14"/>
-      <c r="C14"/>
-      <c r="D14"/>
-      <c r="E14"/>
-      <c r="F14"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15"/>
-      <c r="B15"/>
-      <c r="C15"/>
-      <c r="D15"/>
-      <c r="E15"/>
-      <c r="F15"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16"/>
-      <c r="B16"/>
-      <c r="C16"/>
-      <c r="D16"/>
-      <c r="E16"/>
-      <c r="F16"/>
-    </row>
-  </sheetData>
-  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" autoFilter="0" pivotTables="0"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>